<commit_message>
fix: :bug: fix pracititioner role title error in the l2 excel file
</commit_message>
<xml_diff>
--- a/input/l2/global.xlsx
+++ b/input/l2/global.xlsx
@@ -177,7 +177,7 @@
     <t xml:space="preserve">Encounter</t>
   </si>
   <si>
-    <t xml:space="preserve">CHE-practitioner</t>
+    <t xml:space="preserve">CHE-Practitioner</t>
   </si>
   <si>
     <t xml:space="preserve">CHE Practitioner</t>
@@ -195,7 +195,7 @@
     <t xml:space="preserve">CHE-practitionerRole</t>
   </si>
   <si>
-    <t xml:space="preserve">CHE Practitioner Role</t>
+    <t xml:space="preserve">CHE PractitionerRole</t>
   </si>
   <si>
     <t xml:space="preserve">CHE Practitioner Role Profile</t>
@@ -5969,7 +5969,7 @@
     <t xml:space="preserve">CHE.B15S2.DE05</t>
   </si>
   <si>
-    <t xml:space="preserve">EmCare.B16S2.DE01</t>
+    <t xml:space="preserve">CHE.B16S2.DE01</t>
   </si>
   <si>
     <t xml:space="preserve">Oedema of both feet</t>
@@ -8040,72 +8040,6 @@
     <cellStyle name="Excel Built-in Neutral" xfId="22"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF81D41A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF333333"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9211E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0563C1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -8178,7 +8112,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="19:19"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.37109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8737,24 +8671,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0"/>
-      <c r="B19" s="0"/>
-      <c r="C19" s="0"/>
-      <c r="D19" s="0"/>
-      <c r="E19" s="0"/>
-      <c r="F19" s="0"/>
-      <c r="G19" s="0"/>
-      <c r="H19" s="0"/>
-      <c r="I19" s="0"/>
-      <c r="J19" s="0"/>
-      <c r="K19" s="0"/>
-      <c r="L19" s="0"/>
-      <c r="M19" s="0"/>
-      <c r="N19" s="0"/>
-      <c r="O19" s="0"/>
-      <c r="P19" s="0"/>
-      <c r="Q19" s="0"/>
-      <c r="R19" s="0"/>
+      <c r="K19" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8780,7 +8697,7 @@
   <dimension ref="A1:AG24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="19:19 D17"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9487,12 +9404,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG83"/>
+  <dimension ref="A1:AMJ83"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="E44" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="E65" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D22" activeCellId="1" sqref="19:19 D22"/>
+      <selection pane="bottomLeft" activeCell="C66" activeCellId="0" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9755,20 +9672,1036 @@
       </c>
       <c r="P11" s="77"/>
     </row>
-    <row r="12" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="63" t="s">
         <v>813</v>
       </c>
+      <c r="B12" s="13"/>
       <c r="C12" s="13" t="s">
         <v>1133</v>
       </c>
-      <c r="D12" s="1"/>
       <c r="E12" s="78"/>
       <c r="F12" s="78"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
       <c r="I12" s="30" t="s">
         <v>1134</v>
       </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
       <c r="P12" s="77"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="13"/>
+      <c r="AC12" s="13"/>
+      <c r="AD12" s="13"/>
+      <c r="AE12" s="13"/>
+      <c r="AF12" s="13"/>
+      <c r="AG12" s="13"/>
+      <c r="AH12" s="13"/>
+      <c r="AI12" s="13"/>
+      <c r="AJ12" s="13"/>
+      <c r="AK12" s="13"/>
+      <c r="AL12" s="13"/>
+      <c r="AM12" s="13"/>
+      <c r="AN12" s="13"/>
+      <c r="AO12" s="13"/>
+      <c r="AP12" s="13"/>
+      <c r="AQ12" s="13"/>
+      <c r="AR12" s="13"/>
+      <c r="AS12" s="13"/>
+      <c r="AT12" s="13"/>
+      <c r="AU12" s="13"/>
+      <c r="AV12" s="13"/>
+      <c r="AW12" s="13"/>
+      <c r="AX12" s="13"/>
+      <c r="AY12" s="13"/>
+      <c r="AZ12" s="13"/>
+      <c r="BA12" s="13"/>
+      <c r="BB12" s="13"/>
+      <c r="BC12" s="13"/>
+      <c r="BD12" s="13"/>
+      <c r="BE12" s="13"/>
+      <c r="BF12" s="13"/>
+      <c r="BG12" s="13"/>
+      <c r="BH12" s="13"/>
+      <c r="BI12" s="13"/>
+      <c r="BJ12" s="13"/>
+      <c r="BK12" s="13"/>
+      <c r="BL12" s="13"/>
+      <c r="BM12" s="13"/>
+      <c r="BN12" s="13"/>
+      <c r="BO12" s="13"/>
+      <c r="BP12" s="13"/>
+      <c r="BQ12" s="13"/>
+      <c r="BR12" s="13"/>
+      <c r="BS12" s="13"/>
+      <c r="BT12" s="13"/>
+      <c r="BU12" s="13"/>
+      <c r="BV12" s="13"/>
+      <c r="BW12" s="13"/>
+      <c r="BX12" s="13"/>
+      <c r="BY12" s="13"/>
+      <c r="BZ12" s="13"/>
+      <c r="CA12" s="13"/>
+      <c r="CB12" s="13"/>
+      <c r="CC12" s="13"/>
+      <c r="CD12" s="13"/>
+      <c r="CE12" s="13"/>
+      <c r="CF12" s="13"/>
+      <c r="CG12" s="13"/>
+      <c r="CH12" s="13"/>
+      <c r="CI12" s="13"/>
+      <c r="CJ12" s="13"/>
+      <c r="CK12" s="13"/>
+      <c r="CL12" s="13"/>
+      <c r="CM12" s="13"/>
+      <c r="CN12" s="13"/>
+      <c r="CO12" s="13"/>
+      <c r="CP12" s="13"/>
+      <c r="CQ12" s="13"/>
+      <c r="CR12" s="13"/>
+      <c r="CS12" s="13"/>
+      <c r="CT12" s="13"/>
+      <c r="CU12" s="13"/>
+      <c r="CV12" s="13"/>
+      <c r="CW12" s="13"/>
+      <c r="CX12" s="13"/>
+      <c r="CY12" s="13"/>
+      <c r="CZ12" s="13"/>
+      <c r="DA12" s="13"/>
+      <c r="DB12" s="13"/>
+      <c r="DC12" s="13"/>
+      <c r="DD12" s="13"/>
+      <c r="DE12" s="13"/>
+      <c r="DF12" s="13"/>
+      <c r="DG12" s="13"/>
+      <c r="DH12" s="13"/>
+      <c r="DI12" s="13"/>
+      <c r="DJ12" s="13"/>
+      <c r="DK12" s="13"/>
+      <c r="DL12" s="13"/>
+      <c r="DM12" s="13"/>
+      <c r="DN12" s="13"/>
+      <c r="DO12" s="13"/>
+      <c r="DP12" s="13"/>
+      <c r="DQ12" s="13"/>
+      <c r="DR12" s="13"/>
+      <c r="DS12" s="13"/>
+      <c r="DT12" s="13"/>
+      <c r="DU12" s="13"/>
+      <c r="DV12" s="13"/>
+      <c r="DW12" s="13"/>
+      <c r="DX12" s="13"/>
+      <c r="DY12" s="13"/>
+      <c r="DZ12" s="13"/>
+      <c r="EA12" s="13"/>
+      <c r="EB12" s="13"/>
+      <c r="EC12" s="13"/>
+      <c r="ED12" s="13"/>
+      <c r="EE12" s="13"/>
+      <c r="EF12" s="13"/>
+      <c r="EG12" s="13"/>
+      <c r="EH12" s="13"/>
+      <c r="EI12" s="13"/>
+      <c r="EJ12" s="13"/>
+      <c r="EK12" s="13"/>
+      <c r="EL12" s="13"/>
+      <c r="EM12" s="13"/>
+      <c r="EN12" s="13"/>
+      <c r="EO12" s="13"/>
+      <c r="EP12" s="13"/>
+      <c r="EQ12" s="13"/>
+      <c r="ER12" s="13"/>
+      <c r="ES12" s="13"/>
+      <c r="ET12" s="13"/>
+      <c r="EU12" s="13"/>
+      <c r="EV12" s="13"/>
+      <c r="EW12" s="13"/>
+      <c r="EX12" s="13"/>
+      <c r="EY12" s="13"/>
+      <c r="EZ12" s="13"/>
+      <c r="FA12" s="13"/>
+      <c r="FB12" s="13"/>
+      <c r="FC12" s="13"/>
+      <c r="FD12" s="13"/>
+      <c r="FE12" s="13"/>
+      <c r="FF12" s="13"/>
+      <c r="FG12" s="13"/>
+      <c r="FH12" s="13"/>
+      <c r="FI12" s="13"/>
+      <c r="FJ12" s="13"/>
+      <c r="FK12" s="13"/>
+      <c r="FL12" s="13"/>
+      <c r="FM12" s="13"/>
+      <c r="FN12" s="13"/>
+      <c r="FO12" s="13"/>
+      <c r="FP12" s="13"/>
+      <c r="FQ12" s="13"/>
+      <c r="FR12" s="13"/>
+      <c r="FS12" s="13"/>
+      <c r="FT12" s="13"/>
+      <c r="FU12" s="13"/>
+      <c r="FV12" s="13"/>
+      <c r="FW12" s="13"/>
+      <c r="FX12" s="13"/>
+      <c r="FY12" s="13"/>
+      <c r="FZ12" s="13"/>
+      <c r="GA12" s="13"/>
+      <c r="GB12" s="13"/>
+      <c r="GC12" s="13"/>
+      <c r="GD12" s="13"/>
+      <c r="GE12" s="13"/>
+      <c r="GF12" s="13"/>
+      <c r="GG12" s="13"/>
+      <c r="GH12" s="13"/>
+      <c r="GI12" s="13"/>
+      <c r="GJ12" s="13"/>
+      <c r="GK12" s="13"/>
+      <c r="GL12" s="13"/>
+      <c r="GM12" s="13"/>
+      <c r="GN12" s="13"/>
+      <c r="GO12" s="13"/>
+      <c r="GP12" s="13"/>
+      <c r="GQ12" s="13"/>
+      <c r="GR12" s="13"/>
+      <c r="GS12" s="13"/>
+      <c r="GT12" s="13"/>
+      <c r="GU12" s="13"/>
+      <c r="GV12" s="13"/>
+      <c r="GW12" s="13"/>
+      <c r="GX12" s="13"/>
+      <c r="GY12" s="13"/>
+      <c r="GZ12" s="13"/>
+      <c r="HA12" s="13"/>
+      <c r="HB12" s="13"/>
+      <c r="HC12" s="13"/>
+      <c r="HD12" s="13"/>
+      <c r="HE12" s="13"/>
+      <c r="HF12" s="13"/>
+      <c r="HG12" s="13"/>
+      <c r="HH12" s="13"/>
+      <c r="HI12" s="13"/>
+      <c r="HJ12" s="13"/>
+      <c r="HK12" s="13"/>
+      <c r="HL12" s="13"/>
+      <c r="HM12" s="13"/>
+      <c r="HN12" s="13"/>
+      <c r="HO12" s="13"/>
+      <c r="HP12" s="13"/>
+      <c r="HQ12" s="13"/>
+      <c r="HR12" s="13"/>
+      <c r="HS12" s="13"/>
+      <c r="HT12" s="13"/>
+      <c r="HU12" s="13"/>
+      <c r="HV12" s="13"/>
+      <c r="HW12" s="13"/>
+      <c r="HX12" s="13"/>
+      <c r="HY12" s="13"/>
+      <c r="HZ12" s="13"/>
+      <c r="IA12" s="13"/>
+      <c r="IB12" s="13"/>
+      <c r="IC12" s="13"/>
+      <c r="ID12" s="13"/>
+      <c r="IE12" s="13"/>
+      <c r="IF12" s="13"/>
+      <c r="IG12" s="13"/>
+      <c r="IH12" s="13"/>
+      <c r="II12" s="13"/>
+      <c r="IJ12" s="13"/>
+      <c r="IK12" s="13"/>
+      <c r="IL12" s="13"/>
+      <c r="IM12" s="13"/>
+      <c r="IN12" s="13"/>
+      <c r="IO12" s="13"/>
+      <c r="IP12" s="13"/>
+      <c r="IQ12" s="13"/>
+      <c r="IR12" s="13"/>
+      <c r="IS12" s="13"/>
+      <c r="IT12" s="13"/>
+      <c r="IU12" s="13"/>
+      <c r="IV12" s="13"/>
+      <c r="IW12" s="13"/>
+      <c r="IX12" s="13"/>
+      <c r="IY12" s="13"/>
+      <c r="IZ12" s="13"/>
+      <c r="JA12" s="13"/>
+      <c r="JB12" s="13"/>
+      <c r="JC12" s="13"/>
+      <c r="JD12" s="13"/>
+      <c r="JE12" s="13"/>
+      <c r="JF12" s="13"/>
+      <c r="JG12" s="13"/>
+      <c r="JH12" s="13"/>
+      <c r="JI12" s="13"/>
+      <c r="JJ12" s="13"/>
+      <c r="JK12" s="13"/>
+      <c r="JL12" s="13"/>
+      <c r="JM12" s="13"/>
+      <c r="JN12" s="13"/>
+      <c r="JO12" s="13"/>
+      <c r="JP12" s="13"/>
+      <c r="JQ12" s="13"/>
+      <c r="JR12" s="13"/>
+      <c r="JS12" s="13"/>
+      <c r="JT12" s="13"/>
+      <c r="JU12" s="13"/>
+      <c r="JV12" s="13"/>
+      <c r="JW12" s="13"/>
+      <c r="JX12" s="13"/>
+      <c r="JY12" s="13"/>
+      <c r="JZ12" s="13"/>
+      <c r="KA12" s="13"/>
+      <c r="KB12" s="13"/>
+      <c r="KC12" s="13"/>
+      <c r="KD12" s="13"/>
+      <c r="KE12" s="13"/>
+      <c r="KF12" s="13"/>
+      <c r="KG12" s="13"/>
+      <c r="KH12" s="13"/>
+      <c r="KI12" s="13"/>
+      <c r="KJ12" s="13"/>
+      <c r="KK12" s="13"/>
+      <c r="KL12" s="13"/>
+      <c r="KM12" s="13"/>
+      <c r="KN12" s="13"/>
+      <c r="KO12" s="13"/>
+      <c r="KP12" s="13"/>
+      <c r="KQ12" s="13"/>
+      <c r="KR12" s="13"/>
+      <c r="KS12" s="13"/>
+      <c r="KT12" s="13"/>
+      <c r="KU12" s="13"/>
+      <c r="KV12" s="13"/>
+      <c r="KW12" s="13"/>
+      <c r="KX12" s="13"/>
+      <c r="KY12" s="13"/>
+      <c r="KZ12" s="13"/>
+      <c r="LA12" s="13"/>
+      <c r="LB12" s="13"/>
+      <c r="LC12" s="13"/>
+      <c r="LD12" s="13"/>
+      <c r="LE12" s="13"/>
+      <c r="LF12" s="13"/>
+      <c r="LG12" s="13"/>
+      <c r="LH12" s="13"/>
+      <c r="LI12" s="13"/>
+      <c r="LJ12" s="13"/>
+      <c r="LK12" s="13"/>
+      <c r="LL12" s="13"/>
+      <c r="LM12" s="13"/>
+      <c r="LN12" s="13"/>
+      <c r="LO12" s="13"/>
+      <c r="LP12" s="13"/>
+      <c r="LQ12" s="13"/>
+      <c r="LR12" s="13"/>
+      <c r="LS12" s="13"/>
+      <c r="LT12" s="13"/>
+      <c r="LU12" s="13"/>
+      <c r="LV12" s="13"/>
+      <c r="LW12" s="13"/>
+      <c r="LX12" s="13"/>
+      <c r="LY12" s="13"/>
+      <c r="LZ12" s="13"/>
+      <c r="MA12" s="13"/>
+      <c r="MB12" s="13"/>
+      <c r="MC12" s="13"/>
+      <c r="MD12" s="13"/>
+      <c r="ME12" s="13"/>
+      <c r="MF12" s="13"/>
+      <c r="MG12" s="13"/>
+      <c r="MH12" s="13"/>
+      <c r="MI12" s="13"/>
+      <c r="MJ12" s="13"/>
+      <c r="MK12" s="13"/>
+      <c r="ML12" s="13"/>
+      <c r="MM12" s="13"/>
+      <c r="MN12" s="13"/>
+      <c r="MO12" s="13"/>
+      <c r="MP12" s="13"/>
+      <c r="MQ12" s="13"/>
+      <c r="MR12" s="13"/>
+      <c r="MS12" s="13"/>
+      <c r="MT12" s="13"/>
+      <c r="MU12" s="13"/>
+      <c r="MV12" s="13"/>
+      <c r="MW12" s="13"/>
+      <c r="MX12" s="13"/>
+      <c r="MY12" s="13"/>
+      <c r="MZ12" s="13"/>
+      <c r="NA12" s="13"/>
+      <c r="NB12" s="13"/>
+      <c r="NC12" s="13"/>
+      <c r="ND12" s="13"/>
+      <c r="NE12" s="13"/>
+      <c r="NF12" s="13"/>
+      <c r="NG12" s="13"/>
+      <c r="NH12" s="13"/>
+      <c r="NI12" s="13"/>
+      <c r="NJ12" s="13"/>
+      <c r="NK12" s="13"/>
+      <c r="NL12" s="13"/>
+      <c r="NM12" s="13"/>
+      <c r="NN12" s="13"/>
+      <c r="NO12" s="13"/>
+      <c r="NP12" s="13"/>
+      <c r="NQ12" s="13"/>
+      <c r="NR12" s="13"/>
+      <c r="NS12" s="13"/>
+      <c r="NT12" s="13"/>
+      <c r="NU12" s="13"/>
+      <c r="NV12" s="13"/>
+      <c r="NW12" s="13"/>
+      <c r="NX12" s="13"/>
+      <c r="NY12" s="13"/>
+      <c r="NZ12" s="13"/>
+      <c r="OA12" s="13"/>
+      <c r="OB12" s="13"/>
+      <c r="OC12" s="13"/>
+      <c r="OD12" s="13"/>
+      <c r="OE12" s="13"/>
+      <c r="OF12" s="13"/>
+      <c r="OG12" s="13"/>
+      <c r="OH12" s="13"/>
+      <c r="OI12" s="13"/>
+      <c r="OJ12" s="13"/>
+      <c r="OK12" s="13"/>
+      <c r="OL12" s="13"/>
+      <c r="OM12" s="13"/>
+      <c r="ON12" s="13"/>
+      <c r="OO12" s="13"/>
+      <c r="OP12" s="13"/>
+      <c r="OQ12" s="13"/>
+      <c r="OR12" s="13"/>
+      <c r="OS12" s="13"/>
+      <c r="OT12" s="13"/>
+      <c r="OU12" s="13"/>
+      <c r="OV12" s="13"/>
+      <c r="OW12" s="13"/>
+      <c r="OX12" s="13"/>
+      <c r="OY12" s="13"/>
+      <c r="OZ12" s="13"/>
+      <c r="PA12" s="13"/>
+      <c r="PB12" s="13"/>
+      <c r="PC12" s="13"/>
+      <c r="PD12" s="13"/>
+      <c r="PE12" s="13"/>
+      <c r="PF12" s="13"/>
+      <c r="PG12" s="13"/>
+      <c r="PH12" s="13"/>
+      <c r="PI12" s="13"/>
+      <c r="PJ12" s="13"/>
+      <c r="PK12" s="13"/>
+      <c r="PL12" s="13"/>
+      <c r="PM12" s="13"/>
+      <c r="PN12" s="13"/>
+      <c r="PO12" s="13"/>
+      <c r="PP12" s="13"/>
+      <c r="PQ12" s="13"/>
+      <c r="PR12" s="13"/>
+      <c r="PS12" s="13"/>
+      <c r="PT12" s="13"/>
+      <c r="PU12" s="13"/>
+      <c r="PV12" s="13"/>
+      <c r="PW12" s="13"/>
+      <c r="PX12" s="13"/>
+      <c r="PY12" s="13"/>
+      <c r="PZ12" s="13"/>
+      <c r="QA12" s="13"/>
+      <c r="QB12" s="13"/>
+      <c r="QC12" s="13"/>
+      <c r="QD12" s="13"/>
+      <c r="QE12" s="13"/>
+      <c r="QF12" s="13"/>
+      <c r="QG12" s="13"/>
+      <c r="QH12" s="13"/>
+      <c r="QI12" s="13"/>
+      <c r="QJ12" s="13"/>
+      <c r="QK12" s="13"/>
+      <c r="QL12" s="13"/>
+      <c r="QM12" s="13"/>
+      <c r="QN12" s="13"/>
+      <c r="QO12" s="13"/>
+      <c r="QP12" s="13"/>
+      <c r="QQ12" s="13"/>
+      <c r="QR12" s="13"/>
+      <c r="QS12" s="13"/>
+      <c r="QT12" s="13"/>
+      <c r="QU12" s="13"/>
+      <c r="QV12" s="13"/>
+      <c r="QW12" s="13"/>
+      <c r="QX12" s="13"/>
+      <c r="QY12" s="13"/>
+      <c r="QZ12" s="13"/>
+      <c r="RA12" s="13"/>
+      <c r="RB12" s="13"/>
+      <c r="RC12" s="13"/>
+      <c r="RD12" s="13"/>
+      <c r="RE12" s="13"/>
+      <c r="RF12" s="13"/>
+      <c r="RG12" s="13"/>
+      <c r="RH12" s="13"/>
+      <c r="RI12" s="13"/>
+      <c r="RJ12" s="13"/>
+      <c r="RK12" s="13"/>
+      <c r="RL12" s="13"/>
+      <c r="RM12" s="13"/>
+      <c r="RN12" s="13"/>
+      <c r="RO12" s="13"/>
+      <c r="RP12" s="13"/>
+      <c r="RQ12" s="13"/>
+      <c r="RR12" s="13"/>
+      <c r="RS12" s="13"/>
+      <c r="RT12" s="13"/>
+      <c r="RU12" s="13"/>
+      <c r="RV12" s="13"/>
+      <c r="RW12" s="13"/>
+      <c r="RX12" s="13"/>
+      <c r="RY12" s="13"/>
+      <c r="RZ12" s="13"/>
+      <c r="SA12" s="13"/>
+      <c r="SB12" s="13"/>
+      <c r="SC12" s="13"/>
+      <c r="SD12" s="13"/>
+      <c r="SE12" s="13"/>
+      <c r="SF12" s="13"/>
+      <c r="SG12" s="13"/>
+      <c r="SH12" s="13"/>
+      <c r="SI12" s="13"/>
+      <c r="SJ12" s="13"/>
+      <c r="SK12" s="13"/>
+      <c r="SL12" s="13"/>
+      <c r="SM12" s="13"/>
+      <c r="SN12" s="13"/>
+      <c r="SO12" s="13"/>
+      <c r="SP12" s="13"/>
+      <c r="SQ12" s="13"/>
+      <c r="SR12" s="13"/>
+      <c r="SS12" s="13"/>
+      <c r="ST12" s="13"/>
+      <c r="SU12" s="13"/>
+      <c r="SV12" s="13"/>
+      <c r="SW12" s="13"/>
+      <c r="SX12" s="13"/>
+      <c r="SY12" s="13"/>
+      <c r="SZ12" s="13"/>
+      <c r="TA12" s="13"/>
+      <c r="TB12" s="13"/>
+      <c r="TC12" s="13"/>
+      <c r="TD12" s="13"/>
+      <c r="TE12" s="13"/>
+      <c r="TF12" s="13"/>
+      <c r="TG12" s="13"/>
+      <c r="TH12" s="13"/>
+      <c r="TI12" s="13"/>
+      <c r="TJ12" s="13"/>
+      <c r="TK12" s="13"/>
+      <c r="TL12" s="13"/>
+      <c r="TM12" s="13"/>
+      <c r="TN12" s="13"/>
+      <c r="TO12" s="13"/>
+      <c r="TP12" s="13"/>
+      <c r="TQ12" s="13"/>
+      <c r="TR12" s="13"/>
+      <c r="TS12" s="13"/>
+      <c r="TT12" s="13"/>
+      <c r="TU12" s="13"/>
+      <c r="TV12" s="13"/>
+      <c r="TW12" s="13"/>
+      <c r="TX12" s="13"/>
+      <c r="TY12" s="13"/>
+      <c r="TZ12" s="13"/>
+      <c r="UA12" s="13"/>
+      <c r="UB12" s="13"/>
+      <c r="UC12" s="13"/>
+      <c r="UD12" s="13"/>
+      <c r="UE12" s="13"/>
+      <c r="UF12" s="13"/>
+      <c r="UG12" s="13"/>
+      <c r="UH12" s="13"/>
+      <c r="UI12" s="13"/>
+      <c r="UJ12" s="13"/>
+      <c r="UK12" s="13"/>
+      <c r="UL12" s="13"/>
+      <c r="UM12" s="13"/>
+      <c r="UN12" s="13"/>
+      <c r="UO12" s="13"/>
+      <c r="UP12" s="13"/>
+      <c r="UQ12" s="13"/>
+      <c r="UR12" s="13"/>
+      <c r="US12" s="13"/>
+      <c r="UT12" s="13"/>
+      <c r="UU12" s="13"/>
+      <c r="UV12" s="13"/>
+      <c r="UW12" s="13"/>
+      <c r="UX12" s="13"/>
+      <c r="UY12" s="13"/>
+      <c r="UZ12" s="13"/>
+      <c r="VA12" s="13"/>
+      <c r="VB12" s="13"/>
+      <c r="VC12" s="13"/>
+      <c r="VD12" s="13"/>
+      <c r="VE12" s="13"/>
+      <c r="VF12" s="13"/>
+      <c r="VG12" s="13"/>
+      <c r="VH12" s="13"/>
+      <c r="VI12" s="13"/>
+      <c r="VJ12" s="13"/>
+      <c r="VK12" s="13"/>
+      <c r="VL12" s="13"/>
+      <c r="VM12" s="13"/>
+      <c r="VN12" s="13"/>
+      <c r="VO12" s="13"/>
+      <c r="VP12" s="13"/>
+      <c r="VQ12" s="13"/>
+      <c r="VR12" s="13"/>
+      <c r="VS12" s="13"/>
+      <c r="VT12" s="13"/>
+      <c r="VU12" s="13"/>
+      <c r="VV12" s="13"/>
+      <c r="VW12" s="13"/>
+      <c r="VX12" s="13"/>
+      <c r="VY12" s="13"/>
+      <c r="VZ12" s="13"/>
+      <c r="WA12" s="13"/>
+      <c r="WB12" s="13"/>
+      <c r="WC12" s="13"/>
+      <c r="WD12" s="13"/>
+      <c r="WE12" s="13"/>
+      <c r="WF12" s="13"/>
+      <c r="WG12" s="13"/>
+      <c r="WH12" s="13"/>
+      <c r="WI12" s="13"/>
+      <c r="WJ12" s="13"/>
+      <c r="WK12" s="13"/>
+      <c r="WL12" s="13"/>
+      <c r="WM12" s="13"/>
+      <c r="WN12" s="13"/>
+      <c r="WO12" s="13"/>
+      <c r="WP12" s="13"/>
+      <c r="WQ12" s="13"/>
+      <c r="WR12" s="13"/>
+      <c r="WS12" s="13"/>
+      <c r="WT12" s="13"/>
+      <c r="WU12" s="13"/>
+      <c r="WV12" s="13"/>
+      <c r="WW12" s="13"/>
+      <c r="WX12" s="13"/>
+      <c r="WY12" s="13"/>
+      <c r="WZ12" s="13"/>
+      <c r="XA12" s="13"/>
+      <c r="XB12" s="13"/>
+      <c r="XC12" s="13"/>
+      <c r="XD12" s="13"/>
+      <c r="XE12" s="13"/>
+      <c r="XF12" s="13"/>
+      <c r="XG12" s="13"/>
+      <c r="XH12" s="13"/>
+      <c r="XI12" s="13"/>
+      <c r="XJ12" s="13"/>
+      <c r="XK12" s="13"/>
+      <c r="XL12" s="13"/>
+      <c r="XM12" s="13"/>
+      <c r="XN12" s="13"/>
+      <c r="XO12" s="13"/>
+      <c r="XP12" s="13"/>
+      <c r="XQ12" s="13"/>
+      <c r="XR12" s="13"/>
+      <c r="XS12" s="13"/>
+      <c r="XT12" s="13"/>
+      <c r="XU12" s="13"/>
+      <c r="XV12" s="13"/>
+      <c r="XW12" s="13"/>
+      <c r="XX12" s="13"/>
+      <c r="XY12" s="13"/>
+      <c r="XZ12" s="13"/>
+      <c r="YA12" s="13"/>
+      <c r="YB12" s="13"/>
+      <c r="YC12" s="13"/>
+      <c r="YD12" s="13"/>
+      <c r="YE12" s="13"/>
+      <c r="YF12" s="13"/>
+      <c r="YG12" s="13"/>
+      <c r="YH12" s="13"/>
+      <c r="YI12" s="13"/>
+      <c r="YJ12" s="13"/>
+      <c r="YK12" s="13"/>
+      <c r="YL12" s="13"/>
+      <c r="YM12" s="13"/>
+      <c r="YN12" s="13"/>
+      <c r="YO12" s="13"/>
+      <c r="YP12" s="13"/>
+      <c r="YQ12" s="13"/>
+      <c r="YR12" s="13"/>
+      <c r="YS12" s="13"/>
+      <c r="YT12" s="13"/>
+      <c r="YU12" s="13"/>
+      <c r="YV12" s="13"/>
+      <c r="YW12" s="13"/>
+      <c r="YX12" s="13"/>
+      <c r="YY12" s="13"/>
+      <c r="YZ12" s="13"/>
+      <c r="ZA12" s="13"/>
+      <c r="ZB12" s="13"/>
+      <c r="ZC12" s="13"/>
+      <c r="ZD12" s="13"/>
+      <c r="ZE12" s="13"/>
+      <c r="ZF12" s="13"/>
+      <c r="ZG12" s="13"/>
+      <c r="ZH12" s="13"/>
+      <c r="ZI12" s="13"/>
+      <c r="ZJ12" s="13"/>
+      <c r="ZK12" s="13"/>
+      <c r="ZL12" s="13"/>
+      <c r="ZM12" s="13"/>
+      <c r="ZN12" s="13"/>
+      <c r="ZO12" s="13"/>
+      <c r="ZP12" s="13"/>
+      <c r="ZQ12" s="13"/>
+      <c r="ZR12" s="13"/>
+      <c r="ZS12" s="13"/>
+      <c r="ZT12" s="13"/>
+      <c r="ZU12" s="13"/>
+      <c r="ZV12" s="13"/>
+      <c r="ZW12" s="13"/>
+      <c r="ZX12" s="13"/>
+      <c r="ZY12" s="13"/>
+      <c r="ZZ12" s="13"/>
+      <c r="AAA12" s="13"/>
+      <c r="AAB12" s="13"/>
+      <c r="AAC12" s="13"/>
+      <c r="AAD12" s="13"/>
+      <c r="AAE12" s="13"/>
+      <c r="AAF12" s="13"/>
+      <c r="AAG12" s="13"/>
+      <c r="AAH12" s="13"/>
+      <c r="AAI12" s="13"/>
+      <c r="AAJ12" s="13"/>
+      <c r="AAK12" s="13"/>
+      <c r="AAL12" s="13"/>
+      <c r="AAM12" s="13"/>
+      <c r="AAN12" s="13"/>
+      <c r="AAO12" s="13"/>
+      <c r="AAP12" s="13"/>
+      <c r="AAQ12" s="13"/>
+      <c r="AAR12" s="13"/>
+      <c r="AAS12" s="13"/>
+      <c r="AAT12" s="13"/>
+      <c r="AAU12" s="13"/>
+      <c r="AAV12" s="13"/>
+      <c r="AAW12" s="13"/>
+      <c r="AAX12" s="13"/>
+      <c r="AAY12" s="13"/>
+      <c r="AAZ12" s="13"/>
+      <c r="ABA12" s="13"/>
+      <c r="ABB12" s="13"/>
+      <c r="ABC12" s="13"/>
+      <c r="ABD12" s="13"/>
+      <c r="ABE12" s="13"/>
+      <c r="ABF12" s="13"/>
+      <c r="ABG12" s="13"/>
+      <c r="ABH12" s="13"/>
+      <c r="ABI12" s="13"/>
+      <c r="ABJ12" s="13"/>
+      <c r="ABK12" s="13"/>
+      <c r="ABL12" s="13"/>
+      <c r="ABM12" s="13"/>
+      <c r="ABN12" s="13"/>
+      <c r="ABO12" s="13"/>
+      <c r="ABP12" s="13"/>
+      <c r="ABQ12" s="13"/>
+      <c r="ABR12" s="13"/>
+      <c r="ABS12" s="13"/>
+      <c r="ABT12" s="13"/>
+      <c r="ABU12" s="13"/>
+      <c r="ABV12" s="13"/>
+      <c r="ABW12" s="13"/>
+      <c r="ABX12" s="13"/>
+      <c r="ABY12" s="13"/>
+      <c r="ABZ12" s="13"/>
+      <c r="ACA12" s="13"/>
+      <c r="ACB12" s="13"/>
+      <c r="ACC12" s="13"/>
+      <c r="ACD12" s="13"/>
+      <c r="ACE12" s="13"/>
+      <c r="ACF12" s="13"/>
+      <c r="ACG12" s="13"/>
+      <c r="ACH12" s="13"/>
+      <c r="ACI12" s="13"/>
+      <c r="ACJ12" s="13"/>
+      <c r="ACK12" s="13"/>
+      <c r="ACL12" s="13"/>
+      <c r="ACM12" s="13"/>
+      <c r="ACN12" s="13"/>
+      <c r="ACO12" s="13"/>
+      <c r="ACP12" s="13"/>
+      <c r="ACQ12" s="13"/>
+      <c r="ACR12" s="13"/>
+      <c r="ACS12" s="13"/>
+      <c r="ACT12" s="13"/>
+      <c r="ACU12" s="13"/>
+      <c r="ACV12" s="13"/>
+      <c r="ACW12" s="13"/>
+      <c r="ACX12" s="13"/>
+      <c r="ACY12" s="13"/>
+      <c r="ACZ12" s="13"/>
+      <c r="ADA12" s="13"/>
+      <c r="ADB12" s="13"/>
+      <c r="ADC12" s="13"/>
+      <c r="ADD12" s="13"/>
+      <c r="ADE12" s="13"/>
+      <c r="ADF12" s="13"/>
+      <c r="ADG12" s="13"/>
+      <c r="ADH12" s="13"/>
+      <c r="ADI12" s="13"/>
+      <c r="ADJ12" s="13"/>
+      <c r="ADK12" s="13"/>
+      <c r="ADL12" s="13"/>
+      <c r="ADM12" s="13"/>
+      <c r="ADN12" s="13"/>
+      <c r="ADO12" s="13"/>
+      <c r="ADP12" s="13"/>
+      <c r="ADQ12" s="13"/>
+      <c r="ADR12" s="13"/>
+      <c r="ADS12" s="13"/>
+      <c r="ADT12" s="13"/>
+      <c r="ADU12" s="13"/>
+      <c r="ADV12" s="13"/>
+      <c r="ADW12" s="13"/>
+      <c r="ADX12" s="13"/>
+      <c r="ADY12" s="13"/>
+      <c r="ADZ12" s="13"/>
+      <c r="AEA12" s="13"/>
+      <c r="AEB12" s="13"/>
+      <c r="AEC12" s="13"/>
+      <c r="AED12" s="13"/>
+      <c r="AEE12" s="13"/>
+      <c r="AEF12" s="13"/>
+      <c r="AEG12" s="13"/>
+      <c r="AEH12" s="13"/>
+      <c r="AEI12" s="13"/>
+      <c r="AEJ12" s="13"/>
+      <c r="AEK12" s="13"/>
+      <c r="AEL12" s="13"/>
+      <c r="AEM12" s="13"/>
+      <c r="AEN12" s="13"/>
+      <c r="AEO12" s="13"/>
+      <c r="AEP12" s="13"/>
+      <c r="AEQ12" s="13"/>
+      <c r="AER12" s="13"/>
+      <c r="AES12" s="13"/>
+      <c r="AET12" s="13"/>
+      <c r="AEU12" s="13"/>
+      <c r="AEV12" s="13"/>
+      <c r="AEW12" s="13"/>
+      <c r="AEX12" s="13"/>
+      <c r="AEY12" s="13"/>
+      <c r="AEZ12" s="13"/>
+      <c r="AFA12" s="13"/>
+      <c r="AFB12" s="13"/>
+      <c r="AFC12" s="13"/>
+      <c r="AFD12" s="13"/>
+      <c r="AFE12" s="13"/>
+      <c r="AFF12" s="13"/>
+      <c r="AFG12" s="13"/>
+      <c r="AFH12" s="13"/>
+      <c r="AFI12" s="13"/>
+      <c r="AFJ12" s="13"/>
+      <c r="AFK12" s="13"/>
+      <c r="AFL12" s="13"/>
+      <c r="AFM12" s="13"/>
+      <c r="AFN12" s="13"/>
+      <c r="AFO12" s="13"/>
+      <c r="AFP12" s="13"/>
+      <c r="AFQ12" s="13"/>
+      <c r="AFR12" s="13"/>
+      <c r="AFS12" s="13"/>
+      <c r="AFT12" s="13"/>
+      <c r="AFU12" s="13"/>
+      <c r="AFV12" s="13"/>
+      <c r="AFW12" s="13"/>
+      <c r="AFX12" s="13"/>
+      <c r="AFY12" s="13"/>
+      <c r="AFZ12" s="13"/>
+      <c r="AGA12" s="13"/>
+      <c r="AGB12" s="13"/>
+      <c r="AGC12" s="13"/>
+      <c r="AGD12" s="13"/>
+      <c r="AGE12" s="13"/>
+      <c r="AGF12" s="13"/>
+      <c r="AGG12" s="13"/>
+      <c r="AGH12" s="13"/>
+      <c r="AGI12" s="13"/>
+      <c r="AGJ12" s="13"/>
+      <c r="AGK12" s="13"/>
+      <c r="AGL12" s="13"/>
+      <c r="AGM12" s="13"/>
+      <c r="AGN12" s="13"/>
+      <c r="AGO12" s="13"/>
+      <c r="AGP12" s="13"/>
+      <c r="AGQ12" s="13"/>
+      <c r="AGR12" s="13"/>
+      <c r="AGS12" s="13"/>
+      <c r="AGT12" s="13"/>
+      <c r="AGU12" s="13"/>
+      <c r="AGV12" s="13"/>
+      <c r="AGW12" s="13"/>
+      <c r="AGX12" s="13"/>
+      <c r="AGY12" s="13"/>
+      <c r="AGZ12" s="13"/>
+      <c r="AHA12" s="13"/>
+      <c r="AHB12" s="13"/>
+      <c r="AHC12" s="13"/>
+      <c r="AHD12" s="13"/>
+      <c r="AHE12" s="13"/>
+      <c r="AHF12" s="13"/>
+      <c r="AHG12" s="13"/>
+      <c r="AHH12" s="13"/>
+      <c r="AHI12" s="13"/>
+      <c r="AHJ12" s="13"/>
+      <c r="AHK12" s="13"/>
+      <c r="AHL12" s="13"/>
+      <c r="AHM12" s="13"/>
+      <c r="AHN12" s="13"/>
+      <c r="AHO12" s="13"/>
+      <c r="AHP12" s="13"/>
+      <c r="AHQ12" s="13"/>
+      <c r="AHR12" s="13"/>
+      <c r="AHS12" s="13"/>
+      <c r="AHT12" s="13"/>
+      <c r="AHU12" s="13"/>
+      <c r="AHV12" s="13"/>
+      <c r="AHW12" s="13"/>
+      <c r="AHX12" s="13"/>
+      <c r="AHY12" s="13"/>
+      <c r="AHZ12" s="13"/>
+      <c r="AIA12" s="13"/>
+      <c r="AIB12" s="13"/>
+      <c r="AIC12" s="13"/>
+      <c r="AID12" s="13"/>
+      <c r="AIE12" s="13"/>
+      <c r="AIF12" s="13"/>
+      <c r="AIG12" s="13"/>
+      <c r="AIH12" s="13"/>
+      <c r="AII12" s="13"/>
+      <c r="AIJ12" s="13"/>
+      <c r="AIK12" s="13"/>
+      <c r="AIL12" s="13"/>
+      <c r="AIM12" s="13"/>
+      <c r="AIN12" s="13"/>
+      <c r="AIO12" s="13"/>
+      <c r="AIP12" s="13"/>
+      <c r="AIQ12" s="13"/>
+      <c r="AIR12" s="13"/>
+      <c r="AIS12" s="13"/>
+      <c r="AIT12" s="13"/>
+      <c r="AIU12" s="13"/>
+      <c r="AIV12" s="13"/>
+      <c r="AIW12" s="13"/>
+      <c r="AIX12" s="13"/>
+      <c r="AIY12" s="13"/>
+      <c r="AIZ12" s="13"/>
+      <c r="AJA12" s="13"/>
+      <c r="AJB12" s="13"/>
+      <c r="AJC12" s="13"/>
+      <c r="AJD12" s="13"/>
+      <c r="AJE12" s="13"/>
+      <c r="AJF12" s="13"/>
+      <c r="AJG12" s="13"/>
+      <c r="AJH12" s="13"/>
+      <c r="AJI12" s="13"/>
+      <c r="AJJ12" s="13"/>
+      <c r="AJK12" s="13"/>
+      <c r="AJL12" s="13"/>
+      <c r="AJM12" s="13"/>
+      <c r="AJN12" s="13"/>
+      <c r="AJO12" s="13"/>
+      <c r="AJP12" s="13"/>
+      <c r="AJQ12" s="13"/>
+      <c r="AJR12" s="13"/>
+      <c r="AJS12" s="13"/>
+      <c r="AJT12" s="13"/>
+      <c r="AJU12" s="13"/>
+      <c r="AJV12" s="13"/>
+      <c r="AJW12" s="13"/>
+      <c r="AJX12" s="13"/>
+      <c r="AJY12" s="13"/>
+      <c r="AJZ12" s="13"/>
+      <c r="AKA12" s="13"/>
+      <c r="AKB12" s="13"/>
+      <c r="AKC12" s="13"/>
+      <c r="AKD12" s="13"/>
+      <c r="AKE12" s="13"/>
+      <c r="AKF12" s="13"/>
+      <c r="AKG12" s="13"/>
+      <c r="AKH12" s="13"/>
+      <c r="AKI12" s="13"/>
+      <c r="AKJ12" s="13"/>
+      <c r="AKK12" s="13"/>
+      <c r="AKL12" s="13"/>
+      <c r="AKM12" s="13"/>
+      <c r="AKN12" s="13"/>
+      <c r="AKO12" s="13"/>
+      <c r="AKP12" s="13"/>
+      <c r="AKQ12" s="13"/>
+      <c r="AKR12" s="13"/>
+      <c r="AKS12" s="13"/>
+      <c r="AKT12" s="13"/>
+      <c r="AKU12" s="13"/>
+      <c r="AKV12" s="13"/>
+      <c r="AKW12" s="13"/>
+      <c r="AKX12" s="13"/>
+      <c r="AKY12" s="13"/>
+      <c r="AKZ12" s="13"/>
+      <c r="ALA12" s="13"/>
+      <c r="ALB12" s="13"/>
+      <c r="ALC12" s="13"/>
+      <c r="ALD12" s="13"/>
+      <c r="ALE12" s="13"/>
+      <c r="ALF12" s="13"/>
+      <c r="ALG12" s="13"/>
+      <c r="ALH12" s="13"/>
+      <c r="ALI12" s="13"/>
+      <c r="ALJ12" s="13"/>
+      <c r="ALK12" s="13"/>
+      <c r="ALL12" s="13"/>
+      <c r="ALM12" s="13"/>
+      <c r="ALN12" s="13"/>
+      <c r="ALO12" s="13"/>
+      <c r="ALP12" s="13"/>
+      <c r="ALQ12" s="13"/>
+      <c r="ALR12" s="13"/>
+      <c r="ALS12" s="13"/>
+      <c r="ALT12" s="13"/>
+      <c r="ALU12" s="13"/>
+      <c r="ALV12" s="13"/>
+      <c r="ALW12" s="13"/>
+      <c r="ALX12" s="13"/>
+      <c r="ALY12" s="13"/>
+      <c r="ALZ12" s="13"/>
+      <c r="AMA12" s="13"/>
+      <c r="AMB12" s="13"/>
+      <c r="AMC12" s="13"/>
+      <c r="AMD12" s="13"/>
+      <c r="AME12" s="13"/>
+      <c r="AMF12" s="13"/>
+      <c r="AMG12" s="13"/>
+      <c r="AMH12" s="13"/>
+      <c r="AMI12" s="13"/>
+      <c r="AMJ12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -10912,7 +11845,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" s="130" customFormat="true" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>45</v>
       </c>
@@ -10928,18 +11861,1033 @@
       <c r="E53" s="36" t="s">
         <v>1288</v>
       </c>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
       <c r="I53" s="48" t="s">
         <v>1289</v>
       </c>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
       <c r="P53" s="35" t="s">
         <v>872</v>
       </c>
+      <c r="Q53" s="1"/>
       <c r="R53" s="35" t="s">
         <v>19</v>
       </c>
       <c r="S53" s="35" t="s">
         <v>81</v>
       </c>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="1"/>
+      <c r="X53" s="1"/>
+      <c r="Y53" s="1"/>
+      <c r="Z53" s="1"/>
+      <c r="AA53" s="1"/>
+      <c r="AB53" s="1"/>
+      <c r="AC53" s="1"/>
+      <c r="AD53" s="1"/>
+      <c r="AE53" s="1"/>
+      <c r="AF53" s="1"/>
+      <c r="AG53" s="1"/>
+      <c r="AH53" s="1"/>
+      <c r="AI53" s="1"/>
+      <c r="AJ53" s="1"/>
+      <c r="AK53" s="1"/>
+      <c r="AL53" s="1"/>
+      <c r="AM53" s="1"/>
+      <c r="AN53" s="1"/>
+      <c r="AO53" s="1"/>
+      <c r="AP53" s="1"/>
+      <c r="AQ53" s="1"/>
+      <c r="AR53" s="1"/>
+      <c r="AS53" s="1"/>
+      <c r="AT53" s="1"/>
+      <c r="AU53" s="1"/>
+      <c r="AV53" s="1"/>
+      <c r="AW53" s="1"/>
+      <c r="AX53" s="1"/>
+      <c r="AY53" s="1"/>
+      <c r="AZ53" s="1"/>
+      <c r="BA53" s="1"/>
+      <c r="BB53" s="1"/>
+      <c r="BC53" s="1"/>
+      <c r="BD53" s="1"/>
+      <c r="BE53" s="1"/>
+      <c r="BF53" s="1"/>
+      <c r="BG53" s="1"/>
+      <c r="BH53" s="1"/>
+      <c r="BI53" s="1"/>
+      <c r="BJ53" s="1"/>
+      <c r="BK53" s="1"/>
+      <c r="BL53" s="1"/>
+      <c r="BM53" s="1"/>
+      <c r="BN53" s="1"/>
+      <c r="BO53" s="1"/>
+      <c r="BP53" s="1"/>
+      <c r="BQ53" s="1"/>
+      <c r="BR53" s="1"/>
+      <c r="BS53" s="1"/>
+      <c r="BT53" s="1"/>
+      <c r="BU53" s="1"/>
+      <c r="BV53" s="1"/>
+      <c r="BW53" s="1"/>
+      <c r="BX53" s="1"/>
+      <c r="BY53" s="1"/>
+      <c r="BZ53" s="1"/>
+      <c r="CA53" s="1"/>
+      <c r="CB53" s="1"/>
+      <c r="CC53" s="1"/>
+      <c r="CD53" s="1"/>
+      <c r="CE53" s="1"/>
+      <c r="CF53" s="1"/>
+      <c r="CG53" s="1"/>
+      <c r="CH53" s="1"/>
+      <c r="CI53" s="1"/>
+      <c r="CJ53" s="1"/>
+      <c r="CK53" s="1"/>
+      <c r="CL53" s="1"/>
+      <c r="CM53" s="1"/>
+      <c r="CN53" s="1"/>
+      <c r="CO53" s="1"/>
+      <c r="CP53" s="1"/>
+      <c r="CQ53" s="1"/>
+      <c r="CR53" s="1"/>
+      <c r="CS53" s="1"/>
+      <c r="CT53" s="1"/>
+      <c r="CU53" s="1"/>
+      <c r="CV53" s="1"/>
+      <c r="CW53" s="1"/>
+      <c r="CX53" s="1"/>
+      <c r="CY53" s="1"/>
+      <c r="CZ53" s="1"/>
+      <c r="DA53" s="1"/>
+      <c r="DB53" s="1"/>
+      <c r="DC53" s="1"/>
+      <c r="DD53" s="1"/>
+      <c r="DE53" s="1"/>
+      <c r="DF53" s="1"/>
+      <c r="DG53" s="1"/>
+      <c r="DH53" s="1"/>
+      <c r="DI53" s="1"/>
+      <c r="DJ53" s="1"/>
+      <c r="DK53" s="1"/>
+      <c r="DL53" s="1"/>
+      <c r="DM53" s="1"/>
+      <c r="DN53" s="1"/>
+      <c r="DO53" s="1"/>
+      <c r="DP53" s="1"/>
+      <c r="DQ53" s="1"/>
+      <c r="DR53" s="1"/>
+      <c r="DS53" s="1"/>
+      <c r="DT53" s="1"/>
+      <c r="DU53" s="1"/>
+      <c r="DV53" s="1"/>
+      <c r="DW53" s="1"/>
+      <c r="DX53" s="1"/>
+      <c r="DY53" s="1"/>
+      <c r="DZ53" s="1"/>
+      <c r="EA53" s="1"/>
+      <c r="EB53" s="1"/>
+      <c r="EC53" s="1"/>
+      <c r="ED53" s="1"/>
+      <c r="EE53" s="1"/>
+      <c r="EF53" s="1"/>
+      <c r="EG53" s="1"/>
+      <c r="EH53" s="1"/>
+      <c r="EI53" s="1"/>
+      <c r="EJ53" s="1"/>
+      <c r="EK53" s="1"/>
+      <c r="EL53" s="1"/>
+      <c r="EM53" s="1"/>
+      <c r="EN53" s="1"/>
+      <c r="EO53" s="1"/>
+      <c r="EP53" s="1"/>
+      <c r="EQ53" s="1"/>
+      <c r="ER53" s="1"/>
+      <c r="ES53" s="1"/>
+      <c r="ET53" s="1"/>
+      <c r="EU53" s="1"/>
+      <c r="EV53" s="1"/>
+      <c r="EW53" s="1"/>
+      <c r="EX53" s="1"/>
+      <c r="EY53" s="1"/>
+      <c r="EZ53" s="1"/>
+      <c r="FA53" s="1"/>
+      <c r="FB53" s="1"/>
+      <c r="FC53" s="1"/>
+      <c r="FD53" s="1"/>
+      <c r="FE53" s="1"/>
+      <c r="FF53" s="1"/>
+      <c r="FG53" s="1"/>
+      <c r="FH53" s="1"/>
+      <c r="FI53" s="1"/>
+      <c r="FJ53" s="1"/>
+      <c r="FK53" s="1"/>
+      <c r="FL53" s="1"/>
+      <c r="FM53" s="1"/>
+      <c r="FN53" s="1"/>
+      <c r="FO53" s="1"/>
+      <c r="FP53" s="1"/>
+      <c r="FQ53" s="1"/>
+      <c r="FR53" s="1"/>
+      <c r="FS53" s="1"/>
+      <c r="FT53" s="1"/>
+      <c r="FU53" s="1"/>
+      <c r="FV53" s="1"/>
+      <c r="FW53" s="1"/>
+      <c r="FX53" s="1"/>
+      <c r="FY53" s="1"/>
+      <c r="FZ53" s="1"/>
+      <c r="GA53" s="1"/>
+      <c r="GB53" s="1"/>
+      <c r="GC53" s="1"/>
+      <c r="GD53" s="1"/>
+      <c r="GE53" s="1"/>
+      <c r="GF53" s="1"/>
+      <c r="GG53" s="1"/>
+      <c r="GH53" s="1"/>
+      <c r="GI53" s="1"/>
+      <c r="GJ53" s="1"/>
+      <c r="GK53" s="1"/>
+      <c r="GL53" s="1"/>
+      <c r="GM53" s="1"/>
+      <c r="GN53" s="1"/>
+      <c r="GO53" s="1"/>
+      <c r="GP53" s="1"/>
+      <c r="GQ53" s="1"/>
+      <c r="GR53" s="1"/>
+      <c r="GS53" s="1"/>
+      <c r="GT53" s="1"/>
+      <c r="GU53" s="1"/>
+      <c r="GV53" s="1"/>
+      <c r="GW53" s="1"/>
+      <c r="GX53" s="1"/>
+      <c r="GY53" s="1"/>
+      <c r="GZ53" s="1"/>
+      <c r="HA53" s="1"/>
+      <c r="HB53" s="1"/>
+      <c r="HC53" s="1"/>
+      <c r="HD53" s="1"/>
+      <c r="HE53" s="1"/>
+      <c r="HF53" s="1"/>
+      <c r="HG53" s="1"/>
+      <c r="HH53" s="1"/>
+      <c r="HI53" s="1"/>
+      <c r="HJ53" s="1"/>
+      <c r="HK53" s="1"/>
+      <c r="HL53" s="1"/>
+      <c r="HM53" s="1"/>
+      <c r="HN53" s="1"/>
+      <c r="HO53" s="1"/>
+      <c r="HP53" s="1"/>
+      <c r="HQ53" s="1"/>
+      <c r="HR53" s="1"/>
+      <c r="HS53" s="1"/>
+      <c r="HT53" s="1"/>
+      <c r="HU53" s="1"/>
+      <c r="HV53" s="1"/>
+      <c r="HW53" s="1"/>
+      <c r="HX53" s="1"/>
+      <c r="HY53" s="1"/>
+      <c r="HZ53" s="1"/>
+      <c r="IA53" s="1"/>
+      <c r="IB53" s="1"/>
+      <c r="IC53" s="1"/>
+      <c r="ID53" s="1"/>
+      <c r="IE53" s="1"/>
+      <c r="IF53" s="1"/>
+      <c r="IG53" s="1"/>
+      <c r="IH53" s="1"/>
+      <c r="II53" s="1"/>
+      <c r="IJ53" s="1"/>
+      <c r="IK53" s="1"/>
+      <c r="IL53" s="1"/>
+      <c r="IM53" s="1"/>
+      <c r="IN53" s="1"/>
+      <c r="IO53" s="1"/>
+      <c r="IP53" s="1"/>
+      <c r="IQ53" s="1"/>
+      <c r="IR53" s="1"/>
+      <c r="IS53" s="1"/>
+      <c r="IT53" s="1"/>
+      <c r="IU53" s="1"/>
+      <c r="IV53" s="1"/>
+      <c r="IW53" s="1"/>
+      <c r="IX53" s="1"/>
+      <c r="IY53" s="1"/>
+      <c r="IZ53" s="1"/>
+      <c r="JA53" s="1"/>
+      <c r="JB53" s="1"/>
+      <c r="JC53" s="1"/>
+      <c r="JD53" s="1"/>
+      <c r="JE53" s="1"/>
+      <c r="JF53" s="1"/>
+      <c r="JG53" s="1"/>
+      <c r="JH53" s="1"/>
+      <c r="JI53" s="1"/>
+      <c r="JJ53" s="1"/>
+      <c r="JK53" s="1"/>
+      <c r="JL53" s="1"/>
+      <c r="JM53" s="1"/>
+      <c r="JN53" s="1"/>
+      <c r="JO53" s="1"/>
+      <c r="JP53" s="1"/>
+      <c r="JQ53" s="1"/>
+      <c r="JR53" s="1"/>
+      <c r="JS53" s="1"/>
+      <c r="JT53" s="1"/>
+      <c r="JU53" s="1"/>
+      <c r="JV53" s="1"/>
+      <c r="JW53" s="1"/>
+      <c r="JX53" s="1"/>
+      <c r="JY53" s="1"/>
+      <c r="JZ53" s="1"/>
+      <c r="KA53" s="1"/>
+      <c r="KB53" s="1"/>
+      <c r="KC53" s="1"/>
+      <c r="KD53" s="1"/>
+      <c r="KE53" s="1"/>
+      <c r="KF53" s="1"/>
+      <c r="KG53" s="1"/>
+      <c r="KH53" s="1"/>
+      <c r="KI53" s="1"/>
+      <c r="KJ53" s="1"/>
+      <c r="KK53" s="1"/>
+      <c r="KL53" s="1"/>
+      <c r="KM53" s="1"/>
+      <c r="KN53" s="1"/>
+      <c r="KO53" s="1"/>
+      <c r="KP53" s="1"/>
+      <c r="KQ53" s="1"/>
+      <c r="KR53" s="1"/>
+      <c r="KS53" s="1"/>
+      <c r="KT53" s="1"/>
+      <c r="KU53" s="1"/>
+      <c r="KV53" s="1"/>
+      <c r="KW53" s="1"/>
+      <c r="KX53" s="1"/>
+      <c r="KY53" s="1"/>
+      <c r="KZ53" s="1"/>
+      <c r="LA53" s="1"/>
+      <c r="LB53" s="1"/>
+      <c r="LC53" s="1"/>
+      <c r="LD53" s="1"/>
+      <c r="LE53" s="1"/>
+      <c r="LF53" s="1"/>
+      <c r="LG53" s="1"/>
+      <c r="LH53" s="1"/>
+      <c r="LI53" s="1"/>
+      <c r="LJ53" s="1"/>
+      <c r="LK53" s="1"/>
+      <c r="LL53" s="1"/>
+      <c r="LM53" s="1"/>
+      <c r="LN53" s="1"/>
+      <c r="LO53" s="1"/>
+      <c r="LP53" s="1"/>
+      <c r="LQ53" s="1"/>
+      <c r="LR53" s="1"/>
+      <c r="LS53" s="1"/>
+      <c r="LT53" s="1"/>
+      <c r="LU53" s="1"/>
+      <c r="LV53" s="1"/>
+      <c r="LW53" s="1"/>
+      <c r="LX53" s="1"/>
+      <c r="LY53" s="1"/>
+      <c r="LZ53" s="1"/>
+      <c r="MA53" s="1"/>
+      <c r="MB53" s="1"/>
+      <c r="MC53" s="1"/>
+      <c r="MD53" s="1"/>
+      <c r="ME53" s="1"/>
+      <c r="MF53" s="1"/>
+      <c r="MG53" s="1"/>
+      <c r="MH53" s="1"/>
+      <c r="MI53" s="1"/>
+      <c r="MJ53" s="1"/>
+      <c r="MK53" s="1"/>
+      <c r="ML53" s="1"/>
+      <c r="MM53" s="1"/>
+      <c r="MN53" s="1"/>
+      <c r="MO53" s="1"/>
+      <c r="MP53" s="1"/>
+      <c r="MQ53" s="1"/>
+      <c r="MR53" s="1"/>
+      <c r="MS53" s="1"/>
+      <c r="MT53" s="1"/>
+      <c r="MU53" s="1"/>
+      <c r="MV53" s="1"/>
+      <c r="MW53" s="1"/>
+      <c r="MX53" s="1"/>
+      <c r="MY53" s="1"/>
+      <c r="MZ53" s="1"/>
+      <c r="NA53" s="1"/>
+      <c r="NB53" s="1"/>
+      <c r="NC53" s="1"/>
+      <c r="ND53" s="1"/>
+      <c r="NE53" s="1"/>
+      <c r="NF53" s="1"/>
+      <c r="NG53" s="1"/>
+      <c r="NH53" s="1"/>
+      <c r="NI53" s="1"/>
+      <c r="NJ53" s="1"/>
+      <c r="NK53" s="1"/>
+      <c r="NL53" s="1"/>
+      <c r="NM53" s="1"/>
+      <c r="NN53" s="1"/>
+      <c r="NO53" s="1"/>
+      <c r="NP53" s="1"/>
+      <c r="NQ53" s="1"/>
+      <c r="NR53" s="1"/>
+      <c r="NS53" s="1"/>
+      <c r="NT53" s="1"/>
+      <c r="NU53" s="1"/>
+      <c r="NV53" s="1"/>
+      <c r="NW53" s="1"/>
+      <c r="NX53" s="1"/>
+      <c r="NY53" s="1"/>
+      <c r="NZ53" s="1"/>
+      <c r="OA53" s="1"/>
+      <c r="OB53" s="1"/>
+      <c r="OC53" s="1"/>
+      <c r="OD53" s="1"/>
+      <c r="OE53" s="1"/>
+      <c r="OF53" s="1"/>
+      <c r="OG53" s="1"/>
+      <c r="OH53" s="1"/>
+      <c r="OI53" s="1"/>
+      <c r="OJ53" s="1"/>
+      <c r="OK53" s="1"/>
+      <c r="OL53" s="1"/>
+      <c r="OM53" s="1"/>
+      <c r="ON53" s="1"/>
+      <c r="OO53" s="1"/>
+      <c r="OP53" s="1"/>
+      <c r="OQ53" s="1"/>
+      <c r="OR53" s="1"/>
+      <c r="OS53" s="1"/>
+      <c r="OT53" s="1"/>
+      <c r="OU53" s="1"/>
+      <c r="OV53" s="1"/>
+      <c r="OW53" s="1"/>
+      <c r="OX53" s="1"/>
+      <c r="OY53" s="1"/>
+      <c r="OZ53" s="1"/>
+      <c r="PA53" s="1"/>
+      <c r="PB53" s="1"/>
+      <c r="PC53" s="1"/>
+      <c r="PD53" s="1"/>
+      <c r="PE53" s="1"/>
+      <c r="PF53" s="1"/>
+      <c r="PG53" s="1"/>
+      <c r="PH53" s="1"/>
+      <c r="PI53" s="1"/>
+      <c r="PJ53" s="1"/>
+      <c r="PK53" s="1"/>
+      <c r="PL53" s="1"/>
+      <c r="PM53" s="1"/>
+      <c r="PN53" s="1"/>
+      <c r="PO53" s="1"/>
+      <c r="PP53" s="1"/>
+      <c r="PQ53" s="1"/>
+      <c r="PR53" s="1"/>
+      <c r="PS53" s="1"/>
+      <c r="PT53" s="1"/>
+      <c r="PU53" s="1"/>
+      <c r="PV53" s="1"/>
+      <c r="PW53" s="1"/>
+      <c r="PX53" s="1"/>
+      <c r="PY53" s="1"/>
+      <c r="PZ53" s="1"/>
+      <c r="QA53" s="1"/>
+      <c r="QB53" s="1"/>
+      <c r="QC53" s="1"/>
+      <c r="QD53" s="1"/>
+      <c r="QE53" s="1"/>
+      <c r="QF53" s="1"/>
+      <c r="QG53" s="1"/>
+      <c r="QH53" s="1"/>
+      <c r="QI53" s="1"/>
+      <c r="QJ53" s="1"/>
+      <c r="QK53" s="1"/>
+      <c r="QL53" s="1"/>
+      <c r="QM53" s="1"/>
+      <c r="QN53" s="1"/>
+      <c r="QO53" s="1"/>
+      <c r="QP53" s="1"/>
+      <c r="QQ53" s="1"/>
+      <c r="QR53" s="1"/>
+      <c r="QS53" s="1"/>
+      <c r="QT53" s="1"/>
+      <c r="QU53" s="1"/>
+      <c r="QV53" s="1"/>
+      <c r="QW53" s="1"/>
+      <c r="QX53" s="1"/>
+      <c r="QY53" s="1"/>
+      <c r="QZ53" s="1"/>
+      <c r="RA53" s="1"/>
+      <c r="RB53" s="1"/>
+      <c r="RC53" s="1"/>
+      <c r="RD53" s="1"/>
+      <c r="RE53" s="1"/>
+      <c r="RF53" s="1"/>
+      <c r="RG53" s="1"/>
+      <c r="RH53" s="1"/>
+      <c r="RI53" s="1"/>
+      <c r="RJ53" s="1"/>
+      <c r="RK53" s="1"/>
+      <c r="RL53" s="1"/>
+      <c r="RM53" s="1"/>
+      <c r="RN53" s="1"/>
+      <c r="RO53" s="1"/>
+      <c r="RP53" s="1"/>
+      <c r="RQ53" s="1"/>
+      <c r="RR53" s="1"/>
+      <c r="RS53" s="1"/>
+      <c r="RT53" s="1"/>
+      <c r="RU53" s="1"/>
+      <c r="RV53" s="1"/>
+      <c r="RW53" s="1"/>
+      <c r="RX53" s="1"/>
+      <c r="RY53" s="1"/>
+      <c r="RZ53" s="1"/>
+      <c r="SA53" s="1"/>
+      <c r="SB53" s="1"/>
+      <c r="SC53" s="1"/>
+      <c r="SD53" s="1"/>
+      <c r="SE53" s="1"/>
+      <c r="SF53" s="1"/>
+      <c r="SG53" s="1"/>
+      <c r="SH53" s="1"/>
+      <c r="SI53" s="1"/>
+      <c r="SJ53" s="1"/>
+      <c r="SK53" s="1"/>
+      <c r="SL53" s="1"/>
+      <c r="SM53" s="1"/>
+      <c r="SN53" s="1"/>
+      <c r="SO53" s="1"/>
+      <c r="SP53" s="1"/>
+      <c r="SQ53" s="1"/>
+      <c r="SR53" s="1"/>
+      <c r="SS53" s="1"/>
+      <c r="ST53" s="1"/>
+      <c r="SU53" s="1"/>
+      <c r="SV53" s="1"/>
+      <c r="SW53" s="1"/>
+      <c r="SX53" s="1"/>
+      <c r="SY53" s="1"/>
+      <c r="SZ53" s="1"/>
+      <c r="TA53" s="1"/>
+      <c r="TB53" s="1"/>
+      <c r="TC53" s="1"/>
+      <c r="TD53" s="1"/>
+      <c r="TE53" s="1"/>
+      <c r="TF53" s="1"/>
+      <c r="TG53" s="1"/>
+      <c r="TH53" s="1"/>
+      <c r="TI53" s="1"/>
+      <c r="TJ53" s="1"/>
+      <c r="TK53" s="1"/>
+      <c r="TL53" s="1"/>
+      <c r="TM53" s="1"/>
+      <c r="TN53" s="1"/>
+      <c r="TO53" s="1"/>
+      <c r="TP53" s="1"/>
+      <c r="TQ53" s="1"/>
+      <c r="TR53" s="1"/>
+      <c r="TS53" s="1"/>
+      <c r="TT53" s="1"/>
+      <c r="TU53" s="1"/>
+      <c r="TV53" s="1"/>
+      <c r="TW53" s="1"/>
+      <c r="TX53" s="1"/>
+      <c r="TY53" s="1"/>
+      <c r="TZ53" s="1"/>
+      <c r="UA53" s="1"/>
+      <c r="UB53" s="1"/>
+      <c r="UC53" s="1"/>
+      <c r="UD53" s="1"/>
+      <c r="UE53" s="1"/>
+      <c r="UF53" s="1"/>
+      <c r="UG53" s="1"/>
+      <c r="UH53" s="1"/>
+      <c r="UI53" s="1"/>
+      <c r="UJ53" s="1"/>
+      <c r="UK53" s="1"/>
+      <c r="UL53" s="1"/>
+      <c r="UM53" s="1"/>
+      <c r="UN53" s="1"/>
+      <c r="UO53" s="1"/>
+      <c r="UP53" s="1"/>
+      <c r="UQ53" s="1"/>
+      <c r="UR53" s="1"/>
+      <c r="US53" s="1"/>
+      <c r="UT53" s="1"/>
+      <c r="UU53" s="1"/>
+      <c r="UV53" s="1"/>
+      <c r="UW53" s="1"/>
+      <c r="UX53" s="1"/>
+      <c r="UY53" s="1"/>
+      <c r="UZ53" s="1"/>
+      <c r="VA53" s="1"/>
+      <c r="VB53" s="1"/>
+      <c r="VC53" s="1"/>
+      <c r="VD53" s="1"/>
+      <c r="VE53" s="1"/>
+      <c r="VF53" s="1"/>
+      <c r="VG53" s="1"/>
+      <c r="VH53" s="1"/>
+      <c r="VI53" s="1"/>
+      <c r="VJ53" s="1"/>
+      <c r="VK53" s="1"/>
+      <c r="VL53" s="1"/>
+      <c r="VM53" s="1"/>
+      <c r="VN53" s="1"/>
+      <c r="VO53" s="1"/>
+      <c r="VP53" s="1"/>
+      <c r="VQ53" s="1"/>
+      <c r="VR53" s="1"/>
+      <c r="VS53" s="1"/>
+      <c r="VT53" s="1"/>
+      <c r="VU53" s="1"/>
+      <c r="VV53" s="1"/>
+      <c r="VW53" s="1"/>
+      <c r="VX53" s="1"/>
+      <c r="VY53" s="1"/>
+      <c r="VZ53" s="1"/>
+      <c r="WA53" s="1"/>
+      <c r="WB53" s="1"/>
+      <c r="WC53" s="1"/>
+      <c r="WD53" s="1"/>
+      <c r="WE53" s="1"/>
+      <c r="WF53" s="1"/>
+      <c r="WG53" s="1"/>
+      <c r="WH53" s="1"/>
+      <c r="WI53" s="1"/>
+      <c r="WJ53" s="1"/>
+      <c r="WK53" s="1"/>
+      <c r="WL53" s="1"/>
+      <c r="WM53" s="1"/>
+      <c r="WN53" s="1"/>
+      <c r="WO53" s="1"/>
+      <c r="WP53" s="1"/>
+      <c r="WQ53" s="1"/>
+      <c r="WR53" s="1"/>
+      <c r="WS53" s="1"/>
+      <c r="WT53" s="1"/>
+      <c r="WU53" s="1"/>
+      <c r="WV53" s="1"/>
+      <c r="WW53" s="1"/>
+      <c r="WX53" s="1"/>
+      <c r="WY53" s="1"/>
+      <c r="WZ53" s="1"/>
+      <c r="XA53" s="1"/>
+      <c r="XB53" s="1"/>
+      <c r="XC53" s="1"/>
+      <c r="XD53" s="1"/>
+      <c r="XE53" s="1"/>
+      <c r="XF53" s="1"/>
+      <c r="XG53" s="1"/>
+      <c r="XH53" s="1"/>
+      <c r="XI53" s="1"/>
+      <c r="XJ53" s="1"/>
+      <c r="XK53" s="1"/>
+      <c r="XL53" s="1"/>
+      <c r="XM53" s="1"/>
+      <c r="XN53" s="1"/>
+      <c r="XO53" s="1"/>
+      <c r="XP53" s="1"/>
+      <c r="XQ53" s="1"/>
+      <c r="XR53" s="1"/>
+      <c r="XS53" s="1"/>
+      <c r="XT53" s="1"/>
+      <c r="XU53" s="1"/>
+      <c r="XV53" s="1"/>
+      <c r="XW53" s="1"/>
+      <c r="XX53" s="1"/>
+      <c r="XY53" s="1"/>
+      <c r="XZ53" s="1"/>
+      <c r="YA53" s="1"/>
+      <c r="YB53" s="1"/>
+      <c r="YC53" s="1"/>
+      <c r="YD53" s="1"/>
+      <c r="YE53" s="1"/>
+      <c r="YF53" s="1"/>
+      <c r="YG53" s="1"/>
+      <c r="YH53" s="1"/>
+      <c r="YI53" s="1"/>
+      <c r="YJ53" s="1"/>
+      <c r="YK53" s="1"/>
+      <c r="YL53" s="1"/>
+      <c r="YM53" s="1"/>
+      <c r="YN53" s="1"/>
+      <c r="YO53" s="1"/>
+      <c r="YP53" s="1"/>
+      <c r="YQ53" s="1"/>
+      <c r="YR53" s="1"/>
+      <c r="YS53" s="1"/>
+      <c r="YT53" s="1"/>
+      <c r="YU53" s="1"/>
+      <c r="YV53" s="1"/>
+      <c r="YW53" s="1"/>
+      <c r="YX53" s="1"/>
+      <c r="YY53" s="1"/>
+      <c r="YZ53" s="1"/>
+      <c r="ZA53" s="1"/>
+      <c r="ZB53" s="1"/>
+      <c r="ZC53" s="1"/>
+      <c r="ZD53" s="1"/>
+      <c r="ZE53" s="1"/>
+      <c r="ZF53" s="1"/>
+      <c r="ZG53" s="1"/>
+      <c r="ZH53" s="1"/>
+      <c r="ZI53" s="1"/>
+      <c r="ZJ53" s="1"/>
+      <c r="ZK53" s="1"/>
+      <c r="ZL53" s="1"/>
+      <c r="ZM53" s="1"/>
+      <c r="ZN53" s="1"/>
+      <c r="ZO53" s="1"/>
+      <c r="ZP53" s="1"/>
+      <c r="ZQ53" s="1"/>
+      <c r="ZR53" s="1"/>
+      <c r="ZS53" s="1"/>
+      <c r="ZT53" s="1"/>
+      <c r="ZU53" s="1"/>
+      <c r="ZV53" s="1"/>
+      <c r="ZW53" s="1"/>
+      <c r="ZX53" s="1"/>
+      <c r="ZY53" s="1"/>
+      <c r="ZZ53" s="1"/>
+      <c r="AAA53" s="1"/>
+      <c r="AAB53" s="1"/>
+      <c r="AAC53" s="1"/>
+      <c r="AAD53" s="1"/>
+      <c r="AAE53" s="1"/>
+      <c r="AAF53" s="1"/>
+      <c r="AAG53" s="1"/>
+      <c r="AAH53" s="1"/>
+      <c r="AAI53" s="1"/>
+      <c r="AAJ53" s="1"/>
+      <c r="AAK53" s="1"/>
+      <c r="AAL53" s="1"/>
+      <c r="AAM53" s="1"/>
+      <c r="AAN53" s="1"/>
+      <c r="AAO53" s="1"/>
+      <c r="AAP53" s="1"/>
+      <c r="AAQ53" s="1"/>
+      <c r="AAR53" s="1"/>
+      <c r="AAS53" s="1"/>
+      <c r="AAT53" s="1"/>
+      <c r="AAU53" s="1"/>
+      <c r="AAV53" s="1"/>
+      <c r="AAW53" s="1"/>
+      <c r="AAX53" s="1"/>
+      <c r="AAY53" s="1"/>
+      <c r="AAZ53" s="1"/>
+      <c r="ABA53" s="1"/>
+      <c r="ABB53" s="1"/>
+      <c r="ABC53" s="1"/>
+      <c r="ABD53" s="1"/>
+      <c r="ABE53" s="1"/>
+      <c r="ABF53" s="1"/>
+      <c r="ABG53" s="1"/>
+      <c r="ABH53" s="1"/>
+      <c r="ABI53" s="1"/>
+      <c r="ABJ53" s="1"/>
+      <c r="ABK53" s="1"/>
+      <c r="ABL53" s="1"/>
+      <c r="ABM53" s="1"/>
+      <c r="ABN53" s="1"/>
+      <c r="ABO53" s="1"/>
+      <c r="ABP53" s="1"/>
+      <c r="ABQ53" s="1"/>
+      <c r="ABR53" s="1"/>
+      <c r="ABS53" s="1"/>
+      <c r="ABT53" s="1"/>
+      <c r="ABU53" s="1"/>
+      <c r="ABV53" s="1"/>
+      <c r="ABW53" s="1"/>
+      <c r="ABX53" s="1"/>
+      <c r="ABY53" s="1"/>
+      <c r="ABZ53" s="1"/>
+      <c r="ACA53" s="1"/>
+      <c r="ACB53" s="1"/>
+      <c r="ACC53" s="1"/>
+      <c r="ACD53" s="1"/>
+      <c r="ACE53" s="1"/>
+      <c r="ACF53" s="1"/>
+      <c r="ACG53" s="1"/>
+      <c r="ACH53" s="1"/>
+      <c r="ACI53" s="1"/>
+      <c r="ACJ53" s="1"/>
+      <c r="ACK53" s="1"/>
+      <c r="ACL53" s="1"/>
+      <c r="ACM53" s="1"/>
+      <c r="ACN53" s="1"/>
+      <c r="ACO53" s="1"/>
+      <c r="ACP53" s="1"/>
+      <c r="ACQ53" s="1"/>
+      <c r="ACR53" s="1"/>
+      <c r="ACS53" s="1"/>
+      <c r="ACT53" s="1"/>
+      <c r="ACU53" s="1"/>
+      <c r="ACV53" s="1"/>
+      <c r="ACW53" s="1"/>
+      <c r="ACX53" s="1"/>
+      <c r="ACY53" s="1"/>
+      <c r="ACZ53" s="1"/>
+      <c r="ADA53" s="1"/>
+      <c r="ADB53" s="1"/>
+      <c r="ADC53" s="1"/>
+      <c r="ADD53" s="1"/>
+      <c r="ADE53" s="1"/>
+      <c r="ADF53" s="1"/>
+      <c r="ADG53" s="1"/>
+      <c r="ADH53" s="1"/>
+      <c r="ADI53" s="1"/>
+      <c r="ADJ53" s="1"/>
+      <c r="ADK53" s="1"/>
+      <c r="ADL53" s="1"/>
+      <c r="ADM53" s="1"/>
+      <c r="ADN53" s="1"/>
+      <c r="ADO53" s="1"/>
+      <c r="ADP53" s="1"/>
+      <c r="ADQ53" s="1"/>
+      <c r="ADR53" s="1"/>
+      <c r="ADS53" s="1"/>
+      <c r="ADT53" s="1"/>
+      <c r="ADU53" s="1"/>
+      <c r="ADV53" s="1"/>
+      <c r="ADW53" s="1"/>
+      <c r="ADX53" s="1"/>
+      <c r="ADY53" s="1"/>
+      <c r="ADZ53" s="1"/>
+      <c r="AEA53" s="1"/>
+      <c r="AEB53" s="1"/>
+      <c r="AEC53" s="1"/>
+      <c r="AED53" s="1"/>
+      <c r="AEE53" s="1"/>
+      <c r="AEF53" s="1"/>
+      <c r="AEG53" s="1"/>
+      <c r="AEH53" s="1"/>
+      <c r="AEI53" s="1"/>
+      <c r="AEJ53" s="1"/>
+      <c r="AEK53" s="1"/>
+      <c r="AEL53" s="1"/>
+      <c r="AEM53" s="1"/>
+      <c r="AEN53" s="1"/>
+      <c r="AEO53" s="1"/>
+      <c r="AEP53" s="1"/>
+      <c r="AEQ53" s="1"/>
+      <c r="AER53" s="1"/>
+      <c r="AES53" s="1"/>
+      <c r="AET53" s="1"/>
+      <c r="AEU53" s="1"/>
+      <c r="AEV53" s="1"/>
+      <c r="AEW53" s="1"/>
+      <c r="AEX53" s="1"/>
+      <c r="AEY53" s="1"/>
+      <c r="AEZ53" s="1"/>
+      <c r="AFA53" s="1"/>
+      <c r="AFB53" s="1"/>
+      <c r="AFC53" s="1"/>
+      <c r="AFD53" s="1"/>
+      <c r="AFE53" s="1"/>
+      <c r="AFF53" s="1"/>
+      <c r="AFG53" s="1"/>
+      <c r="AFH53" s="1"/>
+      <c r="AFI53" s="1"/>
+      <c r="AFJ53" s="1"/>
+      <c r="AFK53" s="1"/>
+      <c r="AFL53" s="1"/>
+      <c r="AFM53" s="1"/>
+      <c r="AFN53" s="1"/>
+      <c r="AFO53" s="1"/>
+      <c r="AFP53" s="1"/>
+      <c r="AFQ53" s="1"/>
+      <c r="AFR53" s="1"/>
+      <c r="AFS53" s="1"/>
+      <c r="AFT53" s="1"/>
+      <c r="AFU53" s="1"/>
+      <c r="AFV53" s="1"/>
+      <c r="AFW53" s="1"/>
+      <c r="AFX53" s="1"/>
+      <c r="AFY53" s="1"/>
+      <c r="AFZ53" s="1"/>
+      <c r="AGA53" s="1"/>
+      <c r="AGB53" s="1"/>
+      <c r="AGC53" s="1"/>
+      <c r="AGD53" s="1"/>
+      <c r="AGE53" s="1"/>
+      <c r="AGF53" s="1"/>
+      <c r="AGG53" s="1"/>
+      <c r="AGH53" s="1"/>
+      <c r="AGI53" s="1"/>
+      <c r="AGJ53" s="1"/>
+      <c r="AGK53" s="1"/>
+      <c r="AGL53" s="1"/>
+      <c r="AGM53" s="1"/>
+      <c r="AGN53" s="1"/>
+      <c r="AGO53" s="1"/>
+      <c r="AGP53" s="1"/>
+      <c r="AGQ53" s="1"/>
+      <c r="AGR53" s="1"/>
+      <c r="AGS53" s="1"/>
+      <c r="AGT53" s="1"/>
+      <c r="AGU53" s="1"/>
+      <c r="AGV53" s="1"/>
+      <c r="AGW53" s="1"/>
+      <c r="AGX53" s="1"/>
+      <c r="AGY53" s="1"/>
+      <c r="AGZ53" s="1"/>
+      <c r="AHA53" s="1"/>
+      <c r="AHB53" s="1"/>
+      <c r="AHC53" s="1"/>
+      <c r="AHD53" s="1"/>
+      <c r="AHE53" s="1"/>
+      <c r="AHF53" s="1"/>
+      <c r="AHG53" s="1"/>
+      <c r="AHH53" s="1"/>
+      <c r="AHI53" s="1"/>
+      <c r="AHJ53" s="1"/>
+      <c r="AHK53" s="1"/>
+      <c r="AHL53" s="1"/>
+      <c r="AHM53" s="1"/>
+      <c r="AHN53" s="1"/>
+      <c r="AHO53" s="1"/>
+      <c r="AHP53" s="1"/>
+      <c r="AHQ53" s="1"/>
+      <c r="AHR53" s="1"/>
+      <c r="AHS53" s="1"/>
+      <c r="AHT53" s="1"/>
+      <c r="AHU53" s="1"/>
+      <c r="AHV53" s="1"/>
+      <c r="AHW53" s="1"/>
+      <c r="AHX53" s="1"/>
+      <c r="AHY53" s="1"/>
+      <c r="AHZ53" s="1"/>
+      <c r="AIA53" s="1"/>
+      <c r="AIB53" s="1"/>
+      <c r="AIC53" s="1"/>
+      <c r="AID53" s="1"/>
+      <c r="AIE53" s="1"/>
+      <c r="AIF53" s="1"/>
+      <c r="AIG53" s="1"/>
+      <c r="AIH53" s="1"/>
+      <c r="AII53" s="1"/>
+      <c r="AIJ53" s="1"/>
+      <c r="AIK53" s="1"/>
+      <c r="AIL53" s="1"/>
+      <c r="AIM53" s="1"/>
+      <c r="AIN53" s="1"/>
+      <c r="AIO53" s="1"/>
+      <c r="AIP53" s="1"/>
+      <c r="AIQ53" s="1"/>
+      <c r="AIR53" s="1"/>
+      <c r="AIS53" s="1"/>
+      <c r="AIT53" s="1"/>
+      <c r="AIU53" s="1"/>
+      <c r="AIV53" s="1"/>
+      <c r="AIW53" s="1"/>
+      <c r="AIX53" s="1"/>
+      <c r="AIY53" s="1"/>
+      <c r="AIZ53" s="1"/>
+      <c r="AJA53" s="1"/>
+      <c r="AJB53" s="1"/>
+      <c r="AJC53" s="1"/>
+      <c r="AJD53" s="1"/>
+      <c r="AJE53" s="1"/>
+      <c r="AJF53" s="1"/>
+      <c r="AJG53" s="1"/>
+      <c r="AJH53" s="1"/>
+      <c r="AJI53" s="1"/>
+      <c r="AJJ53" s="1"/>
+      <c r="AJK53" s="1"/>
+      <c r="AJL53" s="1"/>
+      <c r="AJM53" s="1"/>
+      <c r="AJN53" s="1"/>
+      <c r="AJO53" s="1"/>
+      <c r="AJP53" s="1"/>
+      <c r="AJQ53" s="1"/>
+      <c r="AJR53" s="1"/>
+      <c r="AJS53" s="1"/>
+      <c r="AJT53" s="1"/>
+      <c r="AJU53" s="1"/>
+      <c r="AJV53" s="1"/>
+      <c r="AJW53" s="1"/>
+      <c r="AJX53" s="1"/>
+      <c r="AJY53" s="1"/>
+      <c r="AJZ53" s="1"/>
+      <c r="AKA53" s="1"/>
+      <c r="AKB53" s="1"/>
+      <c r="AKC53" s="1"/>
+      <c r="AKD53" s="1"/>
+      <c r="AKE53" s="1"/>
+      <c r="AKF53" s="1"/>
+      <c r="AKG53" s="1"/>
+      <c r="AKH53" s="1"/>
+      <c r="AKI53" s="1"/>
+      <c r="AKJ53" s="1"/>
+      <c r="AKK53" s="1"/>
+      <c r="AKL53" s="1"/>
+      <c r="AKM53" s="1"/>
+      <c r="AKN53" s="1"/>
+      <c r="AKO53" s="1"/>
+      <c r="AKP53" s="1"/>
+      <c r="AKQ53" s="1"/>
+      <c r="AKR53" s="1"/>
+      <c r="AKS53" s="1"/>
+      <c r="AKT53" s="1"/>
+      <c r="AKU53" s="1"/>
+      <c r="AKV53" s="1"/>
+      <c r="AKW53" s="1"/>
+      <c r="AKX53" s="1"/>
+      <c r="AKY53" s="1"/>
+      <c r="AKZ53" s="1"/>
+      <c r="ALA53" s="1"/>
+      <c r="ALB53" s="1"/>
+      <c r="ALC53" s="1"/>
+      <c r="ALD53" s="1"/>
+      <c r="ALE53" s="1"/>
+      <c r="ALF53" s="1"/>
+      <c r="ALG53" s="1"/>
+      <c r="ALH53" s="1"/>
+      <c r="ALI53" s="1"/>
+      <c r="ALJ53" s="1"/>
+      <c r="ALK53" s="1"/>
+      <c r="ALL53" s="1"/>
+      <c r="ALM53" s="1"/>
+      <c r="ALN53" s="1"/>
+      <c r="ALO53" s="1"/>
+      <c r="ALP53" s="1"/>
+      <c r="ALQ53" s="1"/>
+      <c r="ALR53" s="1"/>
+      <c r="ALS53" s="1"/>
+      <c r="ALT53" s="1"/>
+      <c r="ALU53" s="1"/>
+      <c r="ALV53" s="1"/>
+      <c r="ALW53" s="1"/>
+      <c r="ALX53" s="1"/>
+      <c r="ALY53" s="1"/>
+      <c r="ALZ53" s="1"/>
+      <c r="AMA53" s="1"/>
+      <c r="AMB53" s="1"/>
+      <c r="AMC53" s="1"/>
+      <c r="AMD53" s="1"/>
+      <c r="AME53" s="1"/>
+      <c r="AMF53" s="1"/>
+      <c r="AMG53" s="1"/>
+      <c r="AMH53" s="1"/>
+      <c r="AMI53" s="1"/>
+      <c r="AMJ53" s="1"/>
     </row>
     <row r="54" s="130" customFormat="true" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="130" t="s">
@@ -10970,7 +12918,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="55" s="130" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="130" t="s">
         <v>45</v>
       </c>
@@ -10986,18 +12934,1033 @@
       <c r="E55" s="134" t="s">
         <v>1295</v>
       </c>
+      <c r="F55" s="130"/>
+      <c r="G55" s="130"/>
+      <c r="H55" s="130"/>
       <c r="I55" s="132" t="s">
         <v>1296</v>
       </c>
+      <c r="J55" s="130"/>
+      <c r="K55" s="130"/>
+      <c r="L55" s="130"/>
+      <c r="M55" s="130"/>
+      <c r="N55" s="130"/>
+      <c r="O55" s="130"/>
       <c r="P55" s="130" t="s">
         <v>872</v>
       </c>
+      <c r="Q55" s="130"/>
       <c r="R55" s="130" t="s">
         <v>19</v>
       </c>
       <c r="S55" s="130" t="s">
         <v>81</v>
       </c>
+      <c r="T55" s="130"/>
+      <c r="U55" s="130"/>
+      <c r="V55" s="130"/>
+      <c r="W55" s="130"/>
+      <c r="X55" s="130"/>
+      <c r="Y55" s="130"/>
+      <c r="Z55" s="130"/>
+      <c r="AA55" s="130"/>
+      <c r="AB55" s="130"/>
+      <c r="AC55" s="130"/>
+      <c r="AD55" s="130"/>
+      <c r="AE55" s="130"/>
+      <c r="AF55" s="130"/>
+      <c r="AG55" s="130"/>
+      <c r="AH55" s="130"/>
+      <c r="AI55" s="130"/>
+      <c r="AJ55" s="130"/>
+      <c r="AK55" s="130"/>
+      <c r="AL55" s="130"/>
+      <c r="AM55" s="130"/>
+      <c r="AN55" s="130"/>
+      <c r="AO55" s="130"/>
+      <c r="AP55" s="130"/>
+      <c r="AQ55" s="130"/>
+      <c r="AR55" s="130"/>
+      <c r="AS55" s="130"/>
+      <c r="AT55" s="130"/>
+      <c r="AU55" s="130"/>
+      <c r="AV55" s="130"/>
+      <c r="AW55" s="130"/>
+      <c r="AX55" s="130"/>
+      <c r="AY55" s="130"/>
+      <c r="AZ55" s="130"/>
+      <c r="BA55" s="130"/>
+      <c r="BB55" s="130"/>
+      <c r="BC55" s="130"/>
+      <c r="BD55" s="130"/>
+      <c r="BE55" s="130"/>
+      <c r="BF55" s="130"/>
+      <c r="BG55" s="130"/>
+      <c r="BH55" s="130"/>
+      <c r="BI55" s="130"/>
+      <c r="BJ55" s="130"/>
+      <c r="BK55" s="130"/>
+      <c r="BL55" s="130"/>
+      <c r="BM55" s="130"/>
+      <c r="BN55" s="130"/>
+      <c r="BO55" s="130"/>
+      <c r="BP55" s="130"/>
+      <c r="BQ55" s="130"/>
+      <c r="BR55" s="130"/>
+      <c r="BS55" s="130"/>
+      <c r="BT55" s="130"/>
+      <c r="BU55" s="130"/>
+      <c r="BV55" s="130"/>
+      <c r="BW55" s="130"/>
+      <c r="BX55" s="130"/>
+      <c r="BY55" s="130"/>
+      <c r="BZ55" s="130"/>
+      <c r="CA55" s="130"/>
+      <c r="CB55" s="130"/>
+      <c r="CC55" s="130"/>
+      <c r="CD55" s="130"/>
+      <c r="CE55" s="130"/>
+      <c r="CF55" s="130"/>
+      <c r="CG55" s="130"/>
+      <c r="CH55" s="130"/>
+      <c r="CI55" s="130"/>
+      <c r="CJ55" s="130"/>
+      <c r="CK55" s="130"/>
+      <c r="CL55" s="130"/>
+      <c r="CM55" s="130"/>
+      <c r="CN55" s="130"/>
+      <c r="CO55" s="130"/>
+      <c r="CP55" s="130"/>
+      <c r="CQ55" s="130"/>
+      <c r="CR55" s="130"/>
+      <c r="CS55" s="130"/>
+      <c r="CT55" s="130"/>
+      <c r="CU55" s="130"/>
+      <c r="CV55" s="130"/>
+      <c r="CW55" s="130"/>
+      <c r="CX55" s="130"/>
+      <c r="CY55" s="130"/>
+      <c r="CZ55" s="130"/>
+      <c r="DA55" s="130"/>
+      <c r="DB55" s="130"/>
+      <c r="DC55" s="130"/>
+      <c r="DD55" s="130"/>
+      <c r="DE55" s="130"/>
+      <c r="DF55" s="130"/>
+      <c r="DG55" s="130"/>
+      <c r="DH55" s="130"/>
+      <c r="DI55" s="130"/>
+      <c r="DJ55" s="130"/>
+      <c r="DK55" s="130"/>
+      <c r="DL55" s="130"/>
+      <c r="DM55" s="130"/>
+      <c r="DN55" s="130"/>
+      <c r="DO55" s="130"/>
+      <c r="DP55" s="130"/>
+      <c r="DQ55" s="130"/>
+      <c r="DR55" s="130"/>
+      <c r="DS55" s="130"/>
+      <c r="DT55" s="130"/>
+      <c r="DU55" s="130"/>
+      <c r="DV55" s="130"/>
+      <c r="DW55" s="130"/>
+      <c r="DX55" s="130"/>
+      <c r="DY55" s="130"/>
+      <c r="DZ55" s="130"/>
+      <c r="EA55" s="130"/>
+      <c r="EB55" s="130"/>
+      <c r="EC55" s="130"/>
+      <c r="ED55" s="130"/>
+      <c r="EE55" s="130"/>
+      <c r="EF55" s="130"/>
+      <c r="EG55" s="130"/>
+      <c r="EH55" s="130"/>
+      <c r="EI55" s="130"/>
+      <c r="EJ55" s="130"/>
+      <c r="EK55" s="130"/>
+      <c r="EL55" s="130"/>
+      <c r="EM55" s="130"/>
+      <c r="EN55" s="130"/>
+      <c r="EO55" s="130"/>
+      <c r="EP55" s="130"/>
+      <c r="EQ55" s="130"/>
+      <c r="ER55" s="130"/>
+      <c r="ES55" s="130"/>
+      <c r="ET55" s="130"/>
+      <c r="EU55" s="130"/>
+      <c r="EV55" s="130"/>
+      <c r="EW55" s="130"/>
+      <c r="EX55" s="130"/>
+      <c r="EY55" s="130"/>
+      <c r="EZ55" s="130"/>
+      <c r="FA55" s="130"/>
+      <c r="FB55" s="130"/>
+      <c r="FC55" s="130"/>
+      <c r="FD55" s="130"/>
+      <c r="FE55" s="130"/>
+      <c r="FF55" s="130"/>
+      <c r="FG55" s="130"/>
+      <c r="FH55" s="130"/>
+      <c r="FI55" s="130"/>
+      <c r="FJ55" s="130"/>
+      <c r="FK55" s="130"/>
+      <c r="FL55" s="130"/>
+      <c r="FM55" s="130"/>
+      <c r="FN55" s="130"/>
+      <c r="FO55" s="130"/>
+      <c r="FP55" s="130"/>
+      <c r="FQ55" s="130"/>
+      <c r="FR55" s="130"/>
+      <c r="FS55" s="130"/>
+      <c r="FT55" s="130"/>
+      <c r="FU55" s="130"/>
+      <c r="FV55" s="130"/>
+      <c r="FW55" s="130"/>
+      <c r="FX55" s="130"/>
+      <c r="FY55" s="130"/>
+      <c r="FZ55" s="130"/>
+      <c r="GA55" s="130"/>
+      <c r="GB55" s="130"/>
+      <c r="GC55" s="130"/>
+      <c r="GD55" s="130"/>
+      <c r="GE55" s="130"/>
+      <c r="GF55" s="130"/>
+      <c r="GG55" s="130"/>
+      <c r="GH55" s="130"/>
+      <c r="GI55" s="130"/>
+      <c r="GJ55" s="130"/>
+      <c r="GK55" s="130"/>
+      <c r="GL55" s="130"/>
+      <c r="GM55" s="130"/>
+      <c r="GN55" s="130"/>
+      <c r="GO55" s="130"/>
+      <c r="GP55" s="130"/>
+      <c r="GQ55" s="130"/>
+      <c r="GR55" s="130"/>
+      <c r="GS55" s="130"/>
+      <c r="GT55" s="130"/>
+      <c r="GU55" s="130"/>
+      <c r="GV55" s="130"/>
+      <c r="GW55" s="130"/>
+      <c r="GX55" s="130"/>
+      <c r="GY55" s="130"/>
+      <c r="GZ55" s="130"/>
+      <c r="HA55" s="130"/>
+      <c r="HB55" s="130"/>
+      <c r="HC55" s="130"/>
+      <c r="HD55" s="130"/>
+      <c r="HE55" s="130"/>
+      <c r="HF55" s="130"/>
+      <c r="HG55" s="130"/>
+      <c r="HH55" s="130"/>
+      <c r="HI55" s="130"/>
+      <c r="HJ55" s="130"/>
+      <c r="HK55" s="130"/>
+      <c r="HL55" s="130"/>
+      <c r="HM55" s="130"/>
+      <c r="HN55" s="130"/>
+      <c r="HO55" s="130"/>
+      <c r="HP55" s="130"/>
+      <c r="HQ55" s="130"/>
+      <c r="HR55" s="130"/>
+      <c r="HS55" s="130"/>
+      <c r="HT55" s="130"/>
+      <c r="HU55" s="130"/>
+      <c r="HV55" s="130"/>
+      <c r="HW55" s="130"/>
+      <c r="HX55" s="130"/>
+      <c r="HY55" s="130"/>
+      <c r="HZ55" s="130"/>
+      <c r="IA55" s="130"/>
+      <c r="IB55" s="130"/>
+      <c r="IC55" s="130"/>
+      <c r="ID55" s="130"/>
+      <c r="IE55" s="130"/>
+      <c r="IF55" s="130"/>
+      <c r="IG55" s="130"/>
+      <c r="IH55" s="130"/>
+      <c r="II55" s="130"/>
+      <c r="IJ55" s="130"/>
+      <c r="IK55" s="130"/>
+      <c r="IL55" s="130"/>
+      <c r="IM55" s="130"/>
+      <c r="IN55" s="130"/>
+      <c r="IO55" s="130"/>
+      <c r="IP55" s="130"/>
+      <c r="IQ55" s="130"/>
+      <c r="IR55" s="130"/>
+      <c r="IS55" s="130"/>
+      <c r="IT55" s="130"/>
+      <c r="IU55" s="130"/>
+      <c r="IV55" s="130"/>
+      <c r="IW55" s="130"/>
+      <c r="IX55" s="130"/>
+      <c r="IY55" s="130"/>
+      <c r="IZ55" s="130"/>
+      <c r="JA55" s="130"/>
+      <c r="JB55" s="130"/>
+      <c r="JC55" s="130"/>
+      <c r="JD55" s="130"/>
+      <c r="JE55" s="130"/>
+      <c r="JF55" s="130"/>
+      <c r="JG55" s="130"/>
+      <c r="JH55" s="130"/>
+      <c r="JI55" s="130"/>
+      <c r="JJ55" s="130"/>
+      <c r="JK55" s="130"/>
+      <c r="JL55" s="130"/>
+      <c r="JM55" s="130"/>
+      <c r="JN55" s="130"/>
+      <c r="JO55" s="130"/>
+      <c r="JP55" s="130"/>
+      <c r="JQ55" s="130"/>
+      <c r="JR55" s="130"/>
+      <c r="JS55" s="130"/>
+      <c r="JT55" s="130"/>
+      <c r="JU55" s="130"/>
+      <c r="JV55" s="130"/>
+      <c r="JW55" s="130"/>
+      <c r="JX55" s="130"/>
+      <c r="JY55" s="130"/>
+      <c r="JZ55" s="130"/>
+      <c r="KA55" s="130"/>
+      <c r="KB55" s="130"/>
+      <c r="KC55" s="130"/>
+      <c r="KD55" s="130"/>
+      <c r="KE55" s="130"/>
+      <c r="KF55" s="130"/>
+      <c r="KG55" s="130"/>
+      <c r="KH55" s="130"/>
+      <c r="KI55" s="130"/>
+      <c r="KJ55" s="130"/>
+      <c r="KK55" s="130"/>
+      <c r="KL55" s="130"/>
+      <c r="KM55" s="130"/>
+      <c r="KN55" s="130"/>
+      <c r="KO55" s="130"/>
+      <c r="KP55" s="130"/>
+      <c r="KQ55" s="130"/>
+      <c r="KR55" s="130"/>
+      <c r="KS55" s="130"/>
+      <c r="KT55" s="130"/>
+      <c r="KU55" s="130"/>
+      <c r="KV55" s="130"/>
+      <c r="KW55" s="130"/>
+      <c r="KX55" s="130"/>
+      <c r="KY55" s="130"/>
+      <c r="KZ55" s="130"/>
+      <c r="LA55" s="130"/>
+      <c r="LB55" s="130"/>
+      <c r="LC55" s="130"/>
+      <c r="LD55" s="130"/>
+      <c r="LE55" s="130"/>
+      <c r="LF55" s="130"/>
+      <c r="LG55" s="130"/>
+      <c r="LH55" s="130"/>
+      <c r="LI55" s="130"/>
+      <c r="LJ55" s="130"/>
+      <c r="LK55" s="130"/>
+      <c r="LL55" s="130"/>
+      <c r="LM55" s="130"/>
+      <c r="LN55" s="130"/>
+      <c r="LO55" s="130"/>
+      <c r="LP55" s="130"/>
+      <c r="LQ55" s="130"/>
+      <c r="LR55" s="130"/>
+      <c r="LS55" s="130"/>
+      <c r="LT55" s="130"/>
+      <c r="LU55" s="130"/>
+      <c r="LV55" s="130"/>
+      <c r="LW55" s="130"/>
+      <c r="LX55" s="130"/>
+      <c r="LY55" s="130"/>
+      <c r="LZ55" s="130"/>
+      <c r="MA55" s="130"/>
+      <c r="MB55" s="130"/>
+      <c r="MC55" s="130"/>
+      <c r="MD55" s="130"/>
+      <c r="ME55" s="130"/>
+      <c r="MF55" s="130"/>
+      <c r="MG55" s="130"/>
+      <c r="MH55" s="130"/>
+      <c r="MI55" s="130"/>
+      <c r="MJ55" s="130"/>
+      <c r="MK55" s="130"/>
+      <c r="ML55" s="130"/>
+      <c r="MM55" s="130"/>
+      <c r="MN55" s="130"/>
+      <c r="MO55" s="130"/>
+      <c r="MP55" s="130"/>
+      <c r="MQ55" s="130"/>
+      <c r="MR55" s="130"/>
+      <c r="MS55" s="130"/>
+      <c r="MT55" s="130"/>
+      <c r="MU55" s="130"/>
+      <c r="MV55" s="130"/>
+      <c r="MW55" s="130"/>
+      <c r="MX55" s="130"/>
+      <c r="MY55" s="130"/>
+      <c r="MZ55" s="130"/>
+      <c r="NA55" s="130"/>
+      <c r="NB55" s="130"/>
+      <c r="NC55" s="130"/>
+      <c r="ND55" s="130"/>
+      <c r="NE55" s="130"/>
+      <c r="NF55" s="130"/>
+      <c r="NG55" s="130"/>
+      <c r="NH55" s="130"/>
+      <c r="NI55" s="130"/>
+      <c r="NJ55" s="130"/>
+      <c r="NK55" s="130"/>
+      <c r="NL55" s="130"/>
+      <c r="NM55" s="130"/>
+      <c r="NN55" s="130"/>
+      <c r="NO55" s="130"/>
+      <c r="NP55" s="130"/>
+      <c r="NQ55" s="130"/>
+      <c r="NR55" s="130"/>
+      <c r="NS55" s="130"/>
+      <c r="NT55" s="130"/>
+      <c r="NU55" s="130"/>
+      <c r="NV55" s="130"/>
+      <c r="NW55" s="130"/>
+      <c r="NX55" s="130"/>
+      <c r="NY55" s="130"/>
+      <c r="NZ55" s="130"/>
+      <c r="OA55" s="130"/>
+      <c r="OB55" s="130"/>
+      <c r="OC55" s="130"/>
+      <c r="OD55" s="130"/>
+      <c r="OE55" s="130"/>
+      <c r="OF55" s="130"/>
+      <c r="OG55" s="130"/>
+      <c r="OH55" s="130"/>
+      <c r="OI55" s="130"/>
+      <c r="OJ55" s="130"/>
+      <c r="OK55" s="130"/>
+      <c r="OL55" s="130"/>
+      <c r="OM55" s="130"/>
+      <c r="ON55" s="130"/>
+      <c r="OO55" s="130"/>
+      <c r="OP55" s="130"/>
+      <c r="OQ55" s="130"/>
+      <c r="OR55" s="130"/>
+      <c r="OS55" s="130"/>
+      <c r="OT55" s="130"/>
+      <c r="OU55" s="130"/>
+      <c r="OV55" s="130"/>
+      <c r="OW55" s="130"/>
+      <c r="OX55" s="130"/>
+      <c r="OY55" s="130"/>
+      <c r="OZ55" s="130"/>
+      <c r="PA55" s="130"/>
+      <c r="PB55" s="130"/>
+      <c r="PC55" s="130"/>
+      <c r="PD55" s="130"/>
+      <c r="PE55" s="130"/>
+      <c r="PF55" s="130"/>
+      <c r="PG55" s="130"/>
+      <c r="PH55" s="130"/>
+      <c r="PI55" s="130"/>
+      <c r="PJ55" s="130"/>
+      <c r="PK55" s="130"/>
+      <c r="PL55" s="130"/>
+      <c r="PM55" s="130"/>
+      <c r="PN55" s="130"/>
+      <c r="PO55" s="130"/>
+      <c r="PP55" s="130"/>
+      <c r="PQ55" s="130"/>
+      <c r="PR55" s="130"/>
+      <c r="PS55" s="130"/>
+      <c r="PT55" s="130"/>
+      <c r="PU55" s="130"/>
+      <c r="PV55" s="130"/>
+      <c r="PW55" s="130"/>
+      <c r="PX55" s="130"/>
+      <c r="PY55" s="130"/>
+      <c r="PZ55" s="130"/>
+      <c r="QA55" s="130"/>
+      <c r="QB55" s="130"/>
+      <c r="QC55" s="130"/>
+      <c r="QD55" s="130"/>
+      <c r="QE55" s="130"/>
+      <c r="QF55" s="130"/>
+      <c r="QG55" s="130"/>
+      <c r="QH55" s="130"/>
+      <c r="QI55" s="130"/>
+      <c r="QJ55" s="130"/>
+      <c r="QK55" s="130"/>
+      <c r="QL55" s="130"/>
+      <c r="QM55" s="130"/>
+      <c r="QN55" s="130"/>
+      <c r="QO55" s="130"/>
+      <c r="QP55" s="130"/>
+      <c r="QQ55" s="130"/>
+      <c r="QR55" s="130"/>
+      <c r="QS55" s="130"/>
+      <c r="QT55" s="130"/>
+      <c r="QU55" s="130"/>
+      <c r="QV55" s="130"/>
+      <c r="QW55" s="130"/>
+      <c r="QX55" s="130"/>
+      <c r="QY55" s="130"/>
+      <c r="QZ55" s="130"/>
+      <c r="RA55" s="130"/>
+      <c r="RB55" s="130"/>
+      <c r="RC55" s="130"/>
+      <c r="RD55" s="130"/>
+      <c r="RE55" s="130"/>
+      <c r="RF55" s="130"/>
+      <c r="RG55" s="130"/>
+      <c r="RH55" s="130"/>
+      <c r="RI55" s="130"/>
+      <c r="RJ55" s="130"/>
+      <c r="RK55" s="130"/>
+      <c r="RL55" s="130"/>
+      <c r="RM55" s="130"/>
+      <c r="RN55" s="130"/>
+      <c r="RO55" s="130"/>
+      <c r="RP55" s="130"/>
+      <c r="RQ55" s="130"/>
+      <c r="RR55" s="130"/>
+      <c r="RS55" s="130"/>
+      <c r="RT55" s="130"/>
+      <c r="RU55" s="130"/>
+      <c r="RV55" s="130"/>
+      <c r="RW55" s="130"/>
+      <c r="RX55" s="130"/>
+      <c r="RY55" s="130"/>
+      <c r="RZ55" s="130"/>
+      <c r="SA55" s="130"/>
+      <c r="SB55" s="130"/>
+      <c r="SC55" s="130"/>
+      <c r="SD55" s="130"/>
+      <c r="SE55" s="130"/>
+      <c r="SF55" s="130"/>
+      <c r="SG55" s="130"/>
+      <c r="SH55" s="130"/>
+      <c r="SI55" s="130"/>
+      <c r="SJ55" s="130"/>
+      <c r="SK55" s="130"/>
+      <c r="SL55" s="130"/>
+      <c r="SM55" s="130"/>
+      <c r="SN55" s="130"/>
+      <c r="SO55" s="130"/>
+      <c r="SP55" s="130"/>
+      <c r="SQ55" s="130"/>
+      <c r="SR55" s="130"/>
+      <c r="SS55" s="130"/>
+      <c r="ST55" s="130"/>
+      <c r="SU55" s="130"/>
+      <c r="SV55" s="130"/>
+      <c r="SW55" s="130"/>
+      <c r="SX55" s="130"/>
+      <c r="SY55" s="130"/>
+      <c r="SZ55" s="130"/>
+      <c r="TA55" s="130"/>
+      <c r="TB55" s="130"/>
+      <c r="TC55" s="130"/>
+      <c r="TD55" s="130"/>
+      <c r="TE55" s="130"/>
+      <c r="TF55" s="130"/>
+      <c r="TG55" s="130"/>
+      <c r="TH55" s="130"/>
+      <c r="TI55" s="130"/>
+      <c r="TJ55" s="130"/>
+      <c r="TK55" s="130"/>
+      <c r="TL55" s="130"/>
+      <c r="TM55" s="130"/>
+      <c r="TN55" s="130"/>
+      <c r="TO55" s="130"/>
+      <c r="TP55" s="130"/>
+      <c r="TQ55" s="130"/>
+      <c r="TR55" s="130"/>
+      <c r="TS55" s="130"/>
+      <c r="TT55" s="130"/>
+      <c r="TU55" s="130"/>
+      <c r="TV55" s="130"/>
+      <c r="TW55" s="130"/>
+      <c r="TX55" s="130"/>
+      <c r="TY55" s="130"/>
+      <c r="TZ55" s="130"/>
+      <c r="UA55" s="130"/>
+      <c r="UB55" s="130"/>
+      <c r="UC55" s="130"/>
+      <c r="UD55" s="130"/>
+      <c r="UE55" s="130"/>
+      <c r="UF55" s="130"/>
+      <c r="UG55" s="130"/>
+      <c r="UH55" s="130"/>
+      <c r="UI55" s="130"/>
+      <c r="UJ55" s="130"/>
+      <c r="UK55" s="130"/>
+      <c r="UL55" s="130"/>
+      <c r="UM55" s="130"/>
+      <c r="UN55" s="130"/>
+      <c r="UO55" s="130"/>
+      <c r="UP55" s="130"/>
+      <c r="UQ55" s="130"/>
+      <c r="UR55" s="130"/>
+      <c r="US55" s="130"/>
+      <c r="UT55" s="130"/>
+      <c r="UU55" s="130"/>
+      <c r="UV55" s="130"/>
+      <c r="UW55" s="130"/>
+      <c r="UX55" s="130"/>
+      <c r="UY55" s="130"/>
+      <c r="UZ55" s="130"/>
+      <c r="VA55" s="130"/>
+      <c r="VB55" s="130"/>
+      <c r="VC55" s="130"/>
+      <c r="VD55" s="130"/>
+      <c r="VE55" s="130"/>
+      <c r="VF55" s="130"/>
+      <c r="VG55" s="130"/>
+      <c r="VH55" s="130"/>
+      <c r="VI55" s="130"/>
+      <c r="VJ55" s="130"/>
+      <c r="VK55" s="130"/>
+      <c r="VL55" s="130"/>
+      <c r="VM55" s="130"/>
+      <c r="VN55" s="130"/>
+      <c r="VO55" s="130"/>
+      <c r="VP55" s="130"/>
+      <c r="VQ55" s="130"/>
+      <c r="VR55" s="130"/>
+      <c r="VS55" s="130"/>
+      <c r="VT55" s="130"/>
+      <c r="VU55" s="130"/>
+      <c r="VV55" s="130"/>
+      <c r="VW55" s="130"/>
+      <c r="VX55" s="130"/>
+      <c r="VY55" s="130"/>
+      <c r="VZ55" s="130"/>
+      <c r="WA55" s="130"/>
+      <c r="WB55" s="130"/>
+      <c r="WC55" s="130"/>
+      <c r="WD55" s="130"/>
+      <c r="WE55" s="130"/>
+      <c r="WF55" s="130"/>
+      <c r="WG55" s="130"/>
+      <c r="WH55" s="130"/>
+      <c r="WI55" s="130"/>
+      <c r="WJ55" s="130"/>
+      <c r="WK55" s="130"/>
+      <c r="WL55" s="130"/>
+      <c r="WM55" s="130"/>
+      <c r="WN55" s="130"/>
+      <c r="WO55" s="130"/>
+      <c r="WP55" s="130"/>
+      <c r="WQ55" s="130"/>
+      <c r="WR55" s="130"/>
+      <c r="WS55" s="130"/>
+      <c r="WT55" s="130"/>
+      <c r="WU55" s="130"/>
+      <c r="WV55" s="130"/>
+      <c r="WW55" s="130"/>
+      <c r="WX55" s="130"/>
+      <c r="WY55" s="130"/>
+      <c r="WZ55" s="130"/>
+      <c r="XA55" s="130"/>
+      <c r="XB55" s="130"/>
+      <c r="XC55" s="130"/>
+      <c r="XD55" s="130"/>
+      <c r="XE55" s="130"/>
+      <c r="XF55" s="130"/>
+      <c r="XG55" s="130"/>
+      <c r="XH55" s="130"/>
+      <c r="XI55" s="130"/>
+      <c r="XJ55" s="130"/>
+      <c r="XK55" s="130"/>
+      <c r="XL55" s="130"/>
+      <c r="XM55" s="130"/>
+      <c r="XN55" s="130"/>
+      <c r="XO55" s="130"/>
+      <c r="XP55" s="130"/>
+      <c r="XQ55" s="130"/>
+      <c r="XR55" s="130"/>
+      <c r="XS55" s="130"/>
+      <c r="XT55" s="130"/>
+      <c r="XU55" s="130"/>
+      <c r="XV55" s="130"/>
+      <c r="XW55" s="130"/>
+      <c r="XX55" s="130"/>
+      <c r="XY55" s="130"/>
+      <c r="XZ55" s="130"/>
+      <c r="YA55" s="130"/>
+      <c r="YB55" s="130"/>
+      <c r="YC55" s="130"/>
+      <c r="YD55" s="130"/>
+      <c r="YE55" s="130"/>
+      <c r="YF55" s="130"/>
+      <c r="YG55" s="130"/>
+      <c r="YH55" s="130"/>
+      <c r="YI55" s="130"/>
+      <c r="YJ55" s="130"/>
+      <c r="YK55" s="130"/>
+      <c r="YL55" s="130"/>
+      <c r="YM55" s="130"/>
+      <c r="YN55" s="130"/>
+      <c r="YO55" s="130"/>
+      <c r="YP55" s="130"/>
+      <c r="YQ55" s="130"/>
+      <c r="YR55" s="130"/>
+      <c r="YS55" s="130"/>
+      <c r="YT55" s="130"/>
+      <c r="YU55" s="130"/>
+      <c r="YV55" s="130"/>
+      <c r="YW55" s="130"/>
+      <c r="YX55" s="130"/>
+      <c r="YY55" s="130"/>
+      <c r="YZ55" s="130"/>
+      <c r="ZA55" s="130"/>
+      <c r="ZB55" s="130"/>
+      <c r="ZC55" s="130"/>
+      <c r="ZD55" s="130"/>
+      <c r="ZE55" s="130"/>
+      <c r="ZF55" s="130"/>
+      <c r="ZG55" s="130"/>
+      <c r="ZH55" s="130"/>
+      <c r="ZI55" s="130"/>
+      <c r="ZJ55" s="130"/>
+      <c r="ZK55" s="130"/>
+      <c r="ZL55" s="130"/>
+      <c r="ZM55" s="130"/>
+      <c r="ZN55" s="130"/>
+      <c r="ZO55" s="130"/>
+      <c r="ZP55" s="130"/>
+      <c r="ZQ55" s="130"/>
+      <c r="ZR55" s="130"/>
+      <c r="ZS55" s="130"/>
+      <c r="ZT55" s="130"/>
+      <c r="ZU55" s="130"/>
+      <c r="ZV55" s="130"/>
+      <c r="ZW55" s="130"/>
+      <c r="ZX55" s="130"/>
+      <c r="ZY55" s="130"/>
+      <c r="ZZ55" s="130"/>
+      <c r="AAA55" s="130"/>
+      <c r="AAB55" s="130"/>
+      <c r="AAC55" s="130"/>
+      <c r="AAD55" s="130"/>
+      <c r="AAE55" s="130"/>
+      <c r="AAF55" s="130"/>
+      <c r="AAG55" s="130"/>
+      <c r="AAH55" s="130"/>
+      <c r="AAI55" s="130"/>
+      <c r="AAJ55" s="130"/>
+      <c r="AAK55" s="130"/>
+      <c r="AAL55" s="130"/>
+      <c r="AAM55" s="130"/>
+      <c r="AAN55" s="130"/>
+      <c r="AAO55" s="130"/>
+      <c r="AAP55" s="130"/>
+      <c r="AAQ55" s="130"/>
+      <c r="AAR55" s="130"/>
+      <c r="AAS55" s="130"/>
+      <c r="AAT55" s="130"/>
+      <c r="AAU55" s="130"/>
+      <c r="AAV55" s="130"/>
+      <c r="AAW55" s="130"/>
+      <c r="AAX55" s="130"/>
+      <c r="AAY55" s="130"/>
+      <c r="AAZ55" s="130"/>
+      <c r="ABA55" s="130"/>
+      <c r="ABB55" s="130"/>
+      <c r="ABC55" s="130"/>
+      <c r="ABD55" s="130"/>
+      <c r="ABE55" s="130"/>
+      <c r="ABF55" s="130"/>
+      <c r="ABG55" s="130"/>
+      <c r="ABH55" s="130"/>
+      <c r="ABI55" s="130"/>
+      <c r="ABJ55" s="130"/>
+      <c r="ABK55" s="130"/>
+      <c r="ABL55" s="130"/>
+      <c r="ABM55" s="130"/>
+      <c r="ABN55" s="130"/>
+      <c r="ABO55" s="130"/>
+      <c r="ABP55" s="130"/>
+      <c r="ABQ55" s="130"/>
+      <c r="ABR55" s="130"/>
+      <c r="ABS55" s="130"/>
+      <c r="ABT55" s="130"/>
+      <c r="ABU55" s="130"/>
+      <c r="ABV55" s="130"/>
+      <c r="ABW55" s="130"/>
+      <c r="ABX55" s="130"/>
+      <c r="ABY55" s="130"/>
+      <c r="ABZ55" s="130"/>
+      <c r="ACA55" s="130"/>
+      <c r="ACB55" s="130"/>
+      <c r="ACC55" s="130"/>
+      <c r="ACD55" s="130"/>
+      <c r="ACE55" s="130"/>
+      <c r="ACF55" s="130"/>
+      <c r="ACG55" s="130"/>
+      <c r="ACH55" s="130"/>
+      <c r="ACI55" s="130"/>
+      <c r="ACJ55" s="130"/>
+      <c r="ACK55" s="130"/>
+      <c r="ACL55" s="130"/>
+      <c r="ACM55" s="130"/>
+      <c r="ACN55" s="130"/>
+      <c r="ACO55" s="130"/>
+      <c r="ACP55" s="130"/>
+      <c r="ACQ55" s="130"/>
+      <c r="ACR55" s="130"/>
+      <c r="ACS55" s="130"/>
+      <c r="ACT55" s="130"/>
+      <c r="ACU55" s="130"/>
+      <c r="ACV55" s="130"/>
+      <c r="ACW55" s="130"/>
+      <c r="ACX55" s="130"/>
+      <c r="ACY55" s="130"/>
+      <c r="ACZ55" s="130"/>
+      <c r="ADA55" s="130"/>
+      <c r="ADB55" s="130"/>
+      <c r="ADC55" s="130"/>
+      <c r="ADD55" s="130"/>
+      <c r="ADE55" s="130"/>
+      <c r="ADF55" s="130"/>
+      <c r="ADG55" s="130"/>
+      <c r="ADH55" s="130"/>
+      <c r="ADI55" s="130"/>
+      <c r="ADJ55" s="130"/>
+      <c r="ADK55" s="130"/>
+      <c r="ADL55" s="130"/>
+      <c r="ADM55" s="130"/>
+      <c r="ADN55" s="130"/>
+      <c r="ADO55" s="130"/>
+      <c r="ADP55" s="130"/>
+      <c r="ADQ55" s="130"/>
+      <c r="ADR55" s="130"/>
+      <c r="ADS55" s="130"/>
+      <c r="ADT55" s="130"/>
+      <c r="ADU55" s="130"/>
+      <c r="ADV55" s="130"/>
+      <c r="ADW55" s="130"/>
+      <c r="ADX55" s="130"/>
+      <c r="ADY55" s="130"/>
+      <c r="ADZ55" s="130"/>
+      <c r="AEA55" s="130"/>
+      <c r="AEB55" s="130"/>
+      <c r="AEC55" s="130"/>
+      <c r="AED55" s="130"/>
+      <c r="AEE55" s="130"/>
+      <c r="AEF55" s="130"/>
+      <c r="AEG55" s="130"/>
+      <c r="AEH55" s="130"/>
+      <c r="AEI55" s="130"/>
+      <c r="AEJ55" s="130"/>
+      <c r="AEK55" s="130"/>
+      <c r="AEL55" s="130"/>
+      <c r="AEM55" s="130"/>
+      <c r="AEN55" s="130"/>
+      <c r="AEO55" s="130"/>
+      <c r="AEP55" s="130"/>
+      <c r="AEQ55" s="130"/>
+      <c r="AER55" s="130"/>
+      <c r="AES55" s="130"/>
+      <c r="AET55" s="130"/>
+      <c r="AEU55" s="130"/>
+      <c r="AEV55" s="130"/>
+      <c r="AEW55" s="130"/>
+      <c r="AEX55" s="130"/>
+      <c r="AEY55" s="130"/>
+      <c r="AEZ55" s="130"/>
+      <c r="AFA55" s="130"/>
+      <c r="AFB55" s="130"/>
+      <c r="AFC55" s="130"/>
+      <c r="AFD55" s="130"/>
+      <c r="AFE55" s="130"/>
+      <c r="AFF55" s="130"/>
+      <c r="AFG55" s="130"/>
+      <c r="AFH55" s="130"/>
+      <c r="AFI55" s="130"/>
+      <c r="AFJ55" s="130"/>
+      <c r="AFK55" s="130"/>
+      <c r="AFL55" s="130"/>
+      <c r="AFM55" s="130"/>
+      <c r="AFN55" s="130"/>
+      <c r="AFO55" s="130"/>
+      <c r="AFP55" s="130"/>
+      <c r="AFQ55" s="130"/>
+      <c r="AFR55" s="130"/>
+      <c r="AFS55" s="130"/>
+      <c r="AFT55" s="130"/>
+      <c r="AFU55" s="130"/>
+      <c r="AFV55" s="130"/>
+      <c r="AFW55" s="130"/>
+      <c r="AFX55" s="130"/>
+      <c r="AFY55" s="130"/>
+      <c r="AFZ55" s="130"/>
+      <c r="AGA55" s="130"/>
+      <c r="AGB55" s="130"/>
+      <c r="AGC55" s="130"/>
+      <c r="AGD55" s="130"/>
+      <c r="AGE55" s="130"/>
+      <c r="AGF55" s="130"/>
+      <c r="AGG55" s="130"/>
+      <c r="AGH55" s="130"/>
+      <c r="AGI55" s="130"/>
+      <c r="AGJ55" s="130"/>
+      <c r="AGK55" s="130"/>
+      <c r="AGL55" s="130"/>
+      <c r="AGM55" s="130"/>
+      <c r="AGN55" s="130"/>
+      <c r="AGO55" s="130"/>
+      <c r="AGP55" s="130"/>
+      <c r="AGQ55" s="130"/>
+      <c r="AGR55" s="130"/>
+      <c r="AGS55" s="130"/>
+      <c r="AGT55" s="130"/>
+      <c r="AGU55" s="130"/>
+      <c r="AGV55" s="130"/>
+      <c r="AGW55" s="130"/>
+      <c r="AGX55" s="130"/>
+      <c r="AGY55" s="130"/>
+      <c r="AGZ55" s="130"/>
+      <c r="AHA55" s="130"/>
+      <c r="AHB55" s="130"/>
+      <c r="AHC55" s="130"/>
+      <c r="AHD55" s="130"/>
+      <c r="AHE55" s="130"/>
+      <c r="AHF55" s="130"/>
+      <c r="AHG55" s="130"/>
+      <c r="AHH55" s="130"/>
+      <c r="AHI55" s="130"/>
+      <c r="AHJ55" s="130"/>
+      <c r="AHK55" s="130"/>
+      <c r="AHL55" s="130"/>
+      <c r="AHM55" s="130"/>
+      <c r="AHN55" s="130"/>
+      <c r="AHO55" s="130"/>
+      <c r="AHP55" s="130"/>
+      <c r="AHQ55" s="130"/>
+      <c r="AHR55" s="130"/>
+      <c r="AHS55" s="130"/>
+      <c r="AHT55" s="130"/>
+      <c r="AHU55" s="130"/>
+      <c r="AHV55" s="130"/>
+      <c r="AHW55" s="130"/>
+      <c r="AHX55" s="130"/>
+      <c r="AHY55" s="130"/>
+      <c r="AHZ55" s="130"/>
+      <c r="AIA55" s="130"/>
+      <c r="AIB55" s="130"/>
+      <c r="AIC55" s="130"/>
+      <c r="AID55" s="130"/>
+      <c r="AIE55" s="130"/>
+      <c r="AIF55" s="130"/>
+      <c r="AIG55" s="130"/>
+      <c r="AIH55" s="130"/>
+      <c r="AII55" s="130"/>
+      <c r="AIJ55" s="130"/>
+      <c r="AIK55" s="130"/>
+      <c r="AIL55" s="130"/>
+      <c r="AIM55" s="130"/>
+      <c r="AIN55" s="130"/>
+      <c r="AIO55" s="130"/>
+      <c r="AIP55" s="130"/>
+      <c r="AIQ55" s="130"/>
+      <c r="AIR55" s="130"/>
+      <c r="AIS55" s="130"/>
+      <c r="AIT55" s="130"/>
+      <c r="AIU55" s="130"/>
+      <c r="AIV55" s="130"/>
+      <c r="AIW55" s="130"/>
+      <c r="AIX55" s="130"/>
+      <c r="AIY55" s="130"/>
+      <c r="AIZ55" s="130"/>
+      <c r="AJA55" s="130"/>
+      <c r="AJB55" s="130"/>
+      <c r="AJC55" s="130"/>
+      <c r="AJD55" s="130"/>
+      <c r="AJE55" s="130"/>
+      <c r="AJF55" s="130"/>
+      <c r="AJG55" s="130"/>
+      <c r="AJH55" s="130"/>
+      <c r="AJI55" s="130"/>
+      <c r="AJJ55" s="130"/>
+      <c r="AJK55" s="130"/>
+      <c r="AJL55" s="130"/>
+      <c r="AJM55" s="130"/>
+      <c r="AJN55" s="130"/>
+      <c r="AJO55" s="130"/>
+      <c r="AJP55" s="130"/>
+      <c r="AJQ55" s="130"/>
+      <c r="AJR55" s="130"/>
+      <c r="AJS55" s="130"/>
+      <c r="AJT55" s="130"/>
+      <c r="AJU55" s="130"/>
+      <c r="AJV55" s="130"/>
+      <c r="AJW55" s="130"/>
+      <c r="AJX55" s="130"/>
+      <c r="AJY55" s="130"/>
+      <c r="AJZ55" s="130"/>
+      <c r="AKA55" s="130"/>
+      <c r="AKB55" s="130"/>
+      <c r="AKC55" s="130"/>
+      <c r="AKD55" s="130"/>
+      <c r="AKE55" s="130"/>
+      <c r="AKF55" s="130"/>
+      <c r="AKG55" s="130"/>
+      <c r="AKH55" s="130"/>
+      <c r="AKI55" s="130"/>
+      <c r="AKJ55" s="130"/>
+      <c r="AKK55" s="130"/>
+      <c r="AKL55" s="130"/>
+      <c r="AKM55" s="130"/>
+      <c r="AKN55" s="130"/>
+      <c r="AKO55" s="130"/>
+      <c r="AKP55" s="130"/>
+      <c r="AKQ55" s="130"/>
+      <c r="AKR55" s="130"/>
+      <c r="AKS55" s="130"/>
+      <c r="AKT55" s="130"/>
+      <c r="AKU55" s="130"/>
+      <c r="AKV55" s="130"/>
+      <c r="AKW55" s="130"/>
+      <c r="AKX55" s="130"/>
+      <c r="AKY55" s="130"/>
+      <c r="AKZ55" s="130"/>
+      <c r="ALA55" s="130"/>
+      <c r="ALB55" s="130"/>
+      <c r="ALC55" s="130"/>
+      <c r="ALD55" s="130"/>
+      <c r="ALE55" s="130"/>
+      <c r="ALF55" s="130"/>
+      <c r="ALG55" s="130"/>
+      <c r="ALH55" s="130"/>
+      <c r="ALI55" s="130"/>
+      <c r="ALJ55" s="130"/>
+      <c r="ALK55" s="130"/>
+      <c r="ALL55" s="130"/>
+      <c r="ALM55" s="130"/>
+      <c r="ALN55" s="130"/>
+      <c r="ALO55" s="130"/>
+      <c r="ALP55" s="130"/>
+      <c r="ALQ55" s="130"/>
+      <c r="ALR55" s="130"/>
+      <c r="ALS55" s="130"/>
+      <c r="ALT55" s="130"/>
+      <c r="ALU55" s="130"/>
+      <c r="ALV55" s="130"/>
+      <c r="ALW55" s="130"/>
+      <c r="ALX55" s="130"/>
+      <c r="ALY55" s="130"/>
+      <c r="ALZ55" s="130"/>
+      <c r="AMA55" s="130"/>
+      <c r="AMB55" s="130"/>
+      <c r="AMC55" s="130"/>
+      <c r="AMD55" s="130"/>
+      <c r="AME55" s="130"/>
+      <c r="AMF55" s="130"/>
+      <c r="AMG55" s="130"/>
+      <c r="AMH55" s="130"/>
+      <c r="AMI55" s="130"/>
+      <c r="AMJ55" s="130"/>
     </row>
     <row r="56" customFormat="false" ht="33.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
@@ -11377,7 +14340,7 @@
   <dimension ref="A1:AG10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AN1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P9" activeCellId="1" sqref="19:19 P9"/>
+      <selection pane="topLeft" activeCell="P9" activeCellId="0" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11627,13 +14590,13 @@
   </sheetPr>
   <dimension ref="A1:AG43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="1" sqref="19:19 D22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="65.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="65.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="59.33"/>
   </cols>
   <sheetData>
@@ -12124,7 +15087,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" s="130" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
@@ -12140,9 +15103,18 @@
       <c r="E23" s="57" t="s">
         <v>1381</v>
       </c>
+      <c r="F23" s="0"/>
+      <c r="G23" s="0"/>
+      <c r="H23" s="0"/>
       <c r="I23" s="57" t="s">
         <v>1382</v>
       </c>
+      <c r="J23" s="0"/>
+      <c r="K23" s="0"/>
+      <c r="L23" s="0"/>
+      <c r="M23" s="0"/>
+      <c r="N23" s="0"/>
+      <c r="O23" s="0"/>
       <c r="P23" s="35" t="s">
         <v>872</v>
       </c>
@@ -12153,6 +15125,20 @@
       <c r="S23" s="35" t="s">
         <v>81</v>
       </c>
+      <c r="T23" s="0"/>
+      <c r="U23" s="0"/>
+      <c r="V23" s="0"/>
+      <c r="W23" s="0"/>
+      <c r="X23" s="0"/>
+      <c r="Y23" s="0"/>
+      <c r="Z23" s="0"/>
+      <c r="AA23" s="0"/>
+      <c r="AB23" s="0"/>
+      <c r="AC23" s="0"/>
+      <c r="AD23" s="0"/>
+      <c r="AE23" s="0"/>
+      <c r="AF23" s="0"/>
+      <c r="AG23" s="0"/>
     </row>
     <row r="24" s="130" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="130" t="s">
@@ -12199,7 +15185,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="26" s="130" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="130" t="s">
         <v>813</v>
       </c>
@@ -12212,9 +15198,35 @@
       <c r="D26" s="59"/>
       <c r="E26" s="59"/>
       <c r="F26" s="1"/>
+      <c r="G26" s="130"/>
+      <c r="H26" s="130"/>
       <c r="I26" s="57" t="s">
         <v>1390</v>
       </c>
+      <c r="J26" s="130"/>
+      <c r="K26" s="130"/>
+      <c r="L26" s="130"/>
+      <c r="M26" s="130"/>
+      <c r="N26" s="130"/>
+      <c r="O26" s="130"/>
+      <c r="P26" s="130"/>
+      <c r="Q26" s="130"/>
+      <c r="R26" s="130"/>
+      <c r="S26" s="130"/>
+      <c r="T26" s="130"/>
+      <c r="U26" s="130"/>
+      <c r="V26" s="130"/>
+      <c r="W26" s="130"/>
+      <c r="X26" s="130"/>
+      <c r="Y26" s="130"/>
+      <c r="Z26" s="130"/>
+      <c r="AA26" s="130"/>
+      <c r="AB26" s="130"/>
+      <c r="AC26" s="130"/>
+      <c r="AD26" s="130"/>
+      <c r="AE26" s="130"/>
+      <c r="AF26" s="130"/>
+      <c r="AG26" s="130"/>
     </row>
     <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="130" t="s">
@@ -12234,7 +15246,7 @@
       </c>
       <c r="I27" s="57"/>
     </row>
-    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" s="130" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="130" t="s">
         <v>884</v>
       </c>
@@ -12248,9 +15260,36 @@
       <c r="E28" s="59" t="s">
         <v>1396</v>
       </c>
+      <c r="F28" s="0"/>
+      <c r="G28" s="0"/>
+      <c r="H28" s="0"/>
       <c r="I28" s="130" t="s">
         <v>1397</v>
       </c>
+      <c r="J28" s="0"/>
+      <c r="K28" s="0"/>
+      <c r="L28" s="0"/>
+      <c r="M28" s="0"/>
+      <c r="N28" s="0"/>
+      <c r="O28" s="0"/>
+      <c r="P28" s="0"/>
+      <c r="Q28" s="0"/>
+      <c r="R28" s="0"/>
+      <c r="S28" s="0"/>
+      <c r="T28" s="0"/>
+      <c r="U28" s="0"/>
+      <c r="V28" s="0"/>
+      <c r="W28" s="0"/>
+      <c r="X28" s="0"/>
+      <c r="Y28" s="0"/>
+      <c r="Z28" s="0"/>
+      <c r="AA28" s="0"/>
+      <c r="AB28" s="0"/>
+      <c r="AC28" s="0"/>
+      <c r="AD28" s="0"/>
+      <c r="AE28" s="0"/>
+      <c r="AF28" s="0"/>
+      <c r="AG28" s="0"/>
     </row>
     <row r="29" s="130" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
@@ -12286,7 +15325,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" s="130" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>884</v>
       </c>
@@ -12303,9 +15342,17 @@
         <v>1402</v>
       </c>
       <c r="F30" s="1"/>
+      <c r="G30" s="130"/>
+      <c r="H30" s="130"/>
       <c r="I30" s="130" t="s">
         <v>1403</v>
       </c>
+      <c r="J30" s="130"/>
+      <c r="K30" s="130"/>
+      <c r="L30" s="130"/>
+      <c r="M30" s="130"/>
+      <c r="N30" s="130"/>
+      <c r="O30" s="130"/>
       <c r="P30" s="35" t="s">
         <v>872</v>
       </c>
@@ -12316,6 +15363,20 @@
       <c r="S30" s="35" t="s">
         <v>81</v>
       </c>
+      <c r="T30" s="130"/>
+      <c r="U30" s="130"/>
+      <c r="V30" s="130"/>
+      <c r="W30" s="130"/>
+      <c r="X30" s="130"/>
+      <c r="Y30" s="130"/>
+      <c r="Z30" s="130"/>
+      <c r="AA30" s="130"/>
+      <c r="AB30" s="130"/>
+      <c r="AC30" s="130"/>
+      <c r="AD30" s="130"/>
+      <c r="AE30" s="130"/>
+      <c r="AF30" s="130"/>
+      <c r="AG30" s="130"/>
     </row>
     <row r="31" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
@@ -12688,7 +15749,7 @@
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="19:19 C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12908,10 +15969,11 @@
         <v>567</v>
       </c>
     </row>
-    <row r="13" s="130" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="130" t="s">
         <v>1458</v>
       </c>
+      <c r="B13" s="130"/>
       <c r="C13" s="59" t="s">
         <v>1461</v>
       </c>
@@ -12921,11 +15983,40 @@
       <c r="E13" s="59" t="s">
         <v>1463</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F13" s="130"/>
+      <c r="G13" s="130"/>
+      <c r="H13" s="130"/>
+      <c r="I13" s="130"/>
+      <c r="J13" s="130"/>
+      <c r="K13" s="130"/>
+      <c r="L13" s="130"/>
+      <c r="M13" s="130"/>
+      <c r="N13" s="130"/>
+      <c r="O13" s="130"/>
+      <c r="P13" s="130"/>
+      <c r="Q13" s="130"/>
+      <c r="R13" s="130"/>
+      <c r="S13" s="130"/>
+      <c r="T13" s="130"/>
+      <c r="U13" s="130"/>
+      <c r="V13" s="130"/>
+      <c r="W13" s="130"/>
+      <c r="X13" s="130"/>
+      <c r="Y13" s="130"/>
+      <c r="Z13" s="130"/>
+      <c r="AA13" s="130"/>
+      <c r="AB13" s="130"/>
+      <c r="AC13" s="130"/>
+      <c r="AD13" s="130"/>
+      <c r="AE13" s="130"/>
+      <c r="AF13" s="130"/>
+      <c r="AG13" s="130"/>
+    </row>
+    <row r="14" s="130" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>576</v>
       </c>
+      <c r="B14" s="0"/>
       <c r="C14" s="57" t="s">
         <v>1464</v>
       </c>
@@ -12935,11 +16026,40 @@
       <c r="E14" s="57" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="15" s="130" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F14" s="0"/>
+      <c r="G14" s="0"/>
+      <c r="H14" s="0"/>
+      <c r="I14" s="0"/>
+      <c r="J14" s="0"/>
+      <c r="K14" s="0"/>
+      <c r="L14" s="0"/>
+      <c r="M14" s="0"/>
+      <c r="N14" s="0"/>
+      <c r="O14" s="0"/>
+      <c r="P14" s="0"/>
+      <c r="Q14" s="0"/>
+      <c r="R14" s="0"/>
+      <c r="S14" s="0"/>
+      <c r="T14" s="0"/>
+      <c r="U14" s="0"/>
+      <c r="V14" s="0"/>
+      <c r="W14" s="0"/>
+      <c r="X14" s="0"/>
+      <c r="Y14" s="0"/>
+      <c r="Z14" s="0"/>
+      <c r="AA14" s="0"/>
+      <c r="AB14" s="0"/>
+      <c r="AC14" s="0"/>
+      <c r="AD14" s="0"/>
+      <c r="AE14" s="0"/>
+      <c r="AF14" s="0"/>
+      <c r="AG14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="130" t="s">
         <v>884</v>
       </c>
+      <c r="B15" s="130"/>
       <c r="C15" s="59" t="s">
         <v>1465</v>
       </c>
@@ -12949,6 +16069,34 @@
       <c r="E15" s="140" t="s">
         <v>1467</v>
       </c>
+      <c r="F15" s="130"/>
+      <c r="G15" s="130"/>
+      <c r="H15" s="130"/>
+      <c r="I15" s="130"/>
+      <c r="J15" s="130"/>
+      <c r="K15" s="130"/>
+      <c r="L15" s="130"/>
+      <c r="M15" s="130"/>
+      <c r="N15" s="130"/>
+      <c r="O15" s="130"/>
+      <c r="P15" s="130"/>
+      <c r="Q15" s="130"/>
+      <c r="R15" s="130"/>
+      <c r="S15" s="130"/>
+      <c r="T15" s="130"/>
+      <c r="U15" s="130"/>
+      <c r="V15" s="130"/>
+      <c r="W15" s="130"/>
+      <c r="X15" s="130"/>
+      <c r="Y15" s="130"/>
+      <c r="Z15" s="130"/>
+      <c r="AA15" s="130"/>
+      <c r="AB15" s="130"/>
+      <c r="AC15" s="130"/>
+      <c r="AD15" s="130"/>
+      <c r="AE15" s="130"/>
+      <c r="AF15" s="130"/>
+      <c r="AG15" s="130"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -12974,7 +16122,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E9" activeCellId="1" sqref="19:19 E9"/>
+      <selection pane="bottomLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13461,7 +16609,7 @@
   <dimension ref="A1:AG9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="1" sqref="19:19 J7"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13857,9 +17005,9 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E126" activeCellId="1" sqref="19:19 E126"/>
+      <selection pane="bottomLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.65234375" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14181,7 +17329,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
         <v>81</v>
       </c>
@@ -14195,8 +17343,11 @@
         <v>130</v>
       </c>
       <c r="E18" s="25"/>
-    </row>
-    <row r="19" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F18" s="0"/>
+      <c r="G18" s="0"/>
+      <c r="H18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
         <v>81</v>
       </c>
@@ -14212,6 +17363,9 @@
       <c r="E19" s="16" t="s">
         <v>133</v>
       </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
@@ -16931,7 +20085,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="19:19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16954,8 +20108,8 @@
   </sheetPr>
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="1" sqref="19:19 D24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17493,10 +20647,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BA65"/>
+  <dimension ref="A1:AMJ65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="19:19 C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28125" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17940,7 +21094,7 @@
       <c r="AB11" s="61"/>
       <c r="AC11" s="61"/>
     </row>
-    <row r="12" s="77" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="61" t="s">
         <v>698</v>
       </c>
@@ -17964,6 +21118,7 @@
       <c r="K12" s="61"/>
       <c r="L12" s="61"/>
       <c r="M12" s="61"/>
+      <c r="N12" s="77"/>
       <c r="O12" s="61"/>
       <c r="P12" s="61"/>
       <c r="Q12" s="61"/>
@@ -18003,6 +21158,977 @@
       <c r="AY12" s="83"/>
       <c r="AZ12" s="83"/>
       <c r="BA12" s="83"/>
+      <c r="BB12" s="77"/>
+      <c r="BC12" s="77"/>
+      <c r="BD12" s="77"/>
+      <c r="BE12" s="77"/>
+      <c r="BF12" s="77"/>
+      <c r="BG12" s="77"/>
+      <c r="BH12" s="77"/>
+      <c r="BI12" s="77"/>
+      <c r="BJ12" s="77"/>
+      <c r="BK12" s="77"/>
+      <c r="BL12" s="77"/>
+      <c r="BM12" s="77"/>
+      <c r="BN12" s="77"/>
+      <c r="BO12" s="77"/>
+      <c r="BP12" s="77"/>
+      <c r="BQ12" s="77"/>
+      <c r="BR12" s="77"/>
+      <c r="BS12" s="77"/>
+      <c r="BT12" s="77"/>
+      <c r="BU12" s="77"/>
+      <c r="BV12" s="77"/>
+      <c r="BW12" s="77"/>
+      <c r="BX12" s="77"/>
+      <c r="BY12" s="77"/>
+      <c r="BZ12" s="77"/>
+      <c r="CA12" s="77"/>
+      <c r="CB12" s="77"/>
+      <c r="CC12" s="77"/>
+      <c r="CD12" s="77"/>
+      <c r="CE12" s="77"/>
+      <c r="CF12" s="77"/>
+      <c r="CG12" s="77"/>
+      <c r="CH12" s="77"/>
+      <c r="CI12" s="77"/>
+      <c r="CJ12" s="77"/>
+      <c r="CK12" s="77"/>
+      <c r="CL12" s="77"/>
+      <c r="CM12" s="77"/>
+      <c r="CN12" s="77"/>
+      <c r="CO12" s="77"/>
+      <c r="CP12" s="77"/>
+      <c r="CQ12" s="77"/>
+      <c r="CR12" s="77"/>
+      <c r="CS12" s="77"/>
+      <c r="CT12" s="77"/>
+      <c r="CU12" s="77"/>
+      <c r="CV12" s="77"/>
+      <c r="CW12" s="77"/>
+      <c r="CX12" s="77"/>
+      <c r="CY12" s="77"/>
+      <c r="CZ12" s="77"/>
+      <c r="DA12" s="77"/>
+      <c r="DB12" s="77"/>
+      <c r="DC12" s="77"/>
+      <c r="DD12" s="77"/>
+      <c r="DE12" s="77"/>
+      <c r="DF12" s="77"/>
+      <c r="DG12" s="77"/>
+      <c r="DH12" s="77"/>
+      <c r="DI12" s="77"/>
+      <c r="DJ12" s="77"/>
+      <c r="DK12" s="77"/>
+      <c r="DL12" s="77"/>
+      <c r="DM12" s="77"/>
+      <c r="DN12" s="77"/>
+      <c r="DO12" s="77"/>
+      <c r="DP12" s="77"/>
+      <c r="DQ12" s="77"/>
+      <c r="DR12" s="77"/>
+      <c r="DS12" s="77"/>
+      <c r="DT12" s="77"/>
+      <c r="DU12" s="77"/>
+      <c r="DV12" s="77"/>
+      <c r="DW12" s="77"/>
+      <c r="DX12" s="77"/>
+      <c r="DY12" s="77"/>
+      <c r="DZ12" s="77"/>
+      <c r="EA12" s="77"/>
+      <c r="EB12" s="77"/>
+      <c r="EC12" s="77"/>
+      <c r="ED12" s="77"/>
+      <c r="EE12" s="77"/>
+      <c r="EF12" s="77"/>
+      <c r="EG12" s="77"/>
+      <c r="EH12" s="77"/>
+      <c r="EI12" s="77"/>
+      <c r="EJ12" s="77"/>
+      <c r="EK12" s="77"/>
+      <c r="EL12" s="77"/>
+      <c r="EM12" s="77"/>
+      <c r="EN12" s="77"/>
+      <c r="EO12" s="77"/>
+      <c r="EP12" s="77"/>
+      <c r="EQ12" s="77"/>
+      <c r="ER12" s="77"/>
+      <c r="ES12" s="77"/>
+      <c r="ET12" s="77"/>
+      <c r="EU12" s="77"/>
+      <c r="EV12" s="77"/>
+      <c r="EW12" s="77"/>
+      <c r="EX12" s="77"/>
+      <c r="EY12" s="77"/>
+      <c r="EZ12" s="77"/>
+      <c r="FA12" s="77"/>
+      <c r="FB12" s="77"/>
+      <c r="FC12" s="77"/>
+      <c r="FD12" s="77"/>
+      <c r="FE12" s="77"/>
+      <c r="FF12" s="77"/>
+      <c r="FG12" s="77"/>
+      <c r="FH12" s="77"/>
+      <c r="FI12" s="77"/>
+      <c r="FJ12" s="77"/>
+      <c r="FK12" s="77"/>
+      <c r="FL12" s="77"/>
+      <c r="FM12" s="77"/>
+      <c r="FN12" s="77"/>
+      <c r="FO12" s="77"/>
+      <c r="FP12" s="77"/>
+      <c r="FQ12" s="77"/>
+      <c r="FR12" s="77"/>
+      <c r="FS12" s="77"/>
+      <c r="FT12" s="77"/>
+      <c r="FU12" s="77"/>
+      <c r="FV12" s="77"/>
+      <c r="FW12" s="77"/>
+      <c r="FX12" s="77"/>
+      <c r="FY12" s="77"/>
+      <c r="FZ12" s="77"/>
+      <c r="GA12" s="77"/>
+      <c r="GB12" s="77"/>
+      <c r="GC12" s="77"/>
+      <c r="GD12" s="77"/>
+      <c r="GE12" s="77"/>
+      <c r="GF12" s="77"/>
+      <c r="GG12" s="77"/>
+      <c r="GH12" s="77"/>
+      <c r="GI12" s="77"/>
+      <c r="GJ12" s="77"/>
+      <c r="GK12" s="77"/>
+      <c r="GL12" s="77"/>
+      <c r="GM12" s="77"/>
+      <c r="GN12" s="77"/>
+      <c r="GO12" s="77"/>
+      <c r="GP12" s="77"/>
+      <c r="GQ12" s="77"/>
+      <c r="GR12" s="77"/>
+      <c r="GS12" s="77"/>
+      <c r="GT12" s="77"/>
+      <c r="GU12" s="77"/>
+      <c r="GV12" s="77"/>
+      <c r="GW12" s="77"/>
+      <c r="GX12" s="77"/>
+      <c r="GY12" s="77"/>
+      <c r="GZ12" s="77"/>
+      <c r="HA12" s="77"/>
+      <c r="HB12" s="77"/>
+      <c r="HC12" s="77"/>
+      <c r="HD12" s="77"/>
+      <c r="HE12" s="77"/>
+      <c r="HF12" s="77"/>
+      <c r="HG12" s="77"/>
+      <c r="HH12" s="77"/>
+      <c r="HI12" s="77"/>
+      <c r="HJ12" s="77"/>
+      <c r="HK12" s="77"/>
+      <c r="HL12" s="77"/>
+      <c r="HM12" s="77"/>
+      <c r="HN12" s="77"/>
+      <c r="HO12" s="77"/>
+      <c r="HP12" s="77"/>
+      <c r="HQ12" s="77"/>
+      <c r="HR12" s="77"/>
+      <c r="HS12" s="77"/>
+      <c r="HT12" s="77"/>
+      <c r="HU12" s="77"/>
+      <c r="HV12" s="77"/>
+      <c r="HW12" s="77"/>
+      <c r="HX12" s="77"/>
+      <c r="HY12" s="77"/>
+      <c r="HZ12" s="77"/>
+      <c r="IA12" s="77"/>
+      <c r="IB12" s="77"/>
+      <c r="IC12" s="77"/>
+      <c r="ID12" s="77"/>
+      <c r="IE12" s="77"/>
+      <c r="IF12" s="77"/>
+      <c r="IG12" s="77"/>
+      <c r="IH12" s="77"/>
+      <c r="II12" s="77"/>
+      <c r="IJ12" s="77"/>
+      <c r="IK12" s="77"/>
+      <c r="IL12" s="77"/>
+      <c r="IM12" s="77"/>
+      <c r="IN12" s="77"/>
+      <c r="IO12" s="77"/>
+      <c r="IP12" s="77"/>
+      <c r="IQ12" s="77"/>
+      <c r="IR12" s="77"/>
+      <c r="IS12" s="77"/>
+      <c r="IT12" s="77"/>
+      <c r="IU12" s="77"/>
+      <c r="IV12" s="77"/>
+      <c r="IW12" s="77"/>
+      <c r="IX12" s="77"/>
+      <c r="IY12" s="77"/>
+      <c r="IZ12" s="77"/>
+      <c r="JA12" s="77"/>
+      <c r="JB12" s="77"/>
+      <c r="JC12" s="77"/>
+      <c r="JD12" s="77"/>
+      <c r="JE12" s="77"/>
+      <c r="JF12" s="77"/>
+      <c r="JG12" s="77"/>
+      <c r="JH12" s="77"/>
+      <c r="JI12" s="77"/>
+      <c r="JJ12" s="77"/>
+      <c r="JK12" s="77"/>
+      <c r="JL12" s="77"/>
+      <c r="JM12" s="77"/>
+      <c r="JN12" s="77"/>
+      <c r="JO12" s="77"/>
+      <c r="JP12" s="77"/>
+      <c r="JQ12" s="77"/>
+      <c r="JR12" s="77"/>
+      <c r="JS12" s="77"/>
+      <c r="JT12" s="77"/>
+      <c r="JU12" s="77"/>
+      <c r="JV12" s="77"/>
+      <c r="JW12" s="77"/>
+      <c r="JX12" s="77"/>
+      <c r="JY12" s="77"/>
+      <c r="JZ12" s="77"/>
+      <c r="KA12" s="77"/>
+      <c r="KB12" s="77"/>
+      <c r="KC12" s="77"/>
+      <c r="KD12" s="77"/>
+      <c r="KE12" s="77"/>
+      <c r="KF12" s="77"/>
+      <c r="KG12" s="77"/>
+      <c r="KH12" s="77"/>
+      <c r="KI12" s="77"/>
+      <c r="KJ12" s="77"/>
+      <c r="KK12" s="77"/>
+      <c r="KL12" s="77"/>
+      <c r="KM12" s="77"/>
+      <c r="KN12" s="77"/>
+      <c r="KO12" s="77"/>
+      <c r="KP12" s="77"/>
+      <c r="KQ12" s="77"/>
+      <c r="KR12" s="77"/>
+      <c r="KS12" s="77"/>
+      <c r="KT12" s="77"/>
+      <c r="KU12" s="77"/>
+      <c r="KV12" s="77"/>
+      <c r="KW12" s="77"/>
+      <c r="KX12" s="77"/>
+      <c r="KY12" s="77"/>
+      <c r="KZ12" s="77"/>
+      <c r="LA12" s="77"/>
+      <c r="LB12" s="77"/>
+      <c r="LC12" s="77"/>
+      <c r="LD12" s="77"/>
+      <c r="LE12" s="77"/>
+      <c r="LF12" s="77"/>
+      <c r="LG12" s="77"/>
+      <c r="LH12" s="77"/>
+      <c r="LI12" s="77"/>
+      <c r="LJ12" s="77"/>
+      <c r="LK12" s="77"/>
+      <c r="LL12" s="77"/>
+      <c r="LM12" s="77"/>
+      <c r="LN12" s="77"/>
+      <c r="LO12" s="77"/>
+      <c r="LP12" s="77"/>
+      <c r="LQ12" s="77"/>
+      <c r="LR12" s="77"/>
+      <c r="LS12" s="77"/>
+      <c r="LT12" s="77"/>
+      <c r="LU12" s="77"/>
+      <c r="LV12" s="77"/>
+      <c r="LW12" s="77"/>
+      <c r="LX12" s="77"/>
+      <c r="LY12" s="77"/>
+      <c r="LZ12" s="77"/>
+      <c r="MA12" s="77"/>
+      <c r="MB12" s="77"/>
+      <c r="MC12" s="77"/>
+      <c r="MD12" s="77"/>
+      <c r="ME12" s="77"/>
+      <c r="MF12" s="77"/>
+      <c r="MG12" s="77"/>
+      <c r="MH12" s="77"/>
+      <c r="MI12" s="77"/>
+      <c r="MJ12" s="77"/>
+      <c r="MK12" s="77"/>
+      <c r="ML12" s="77"/>
+      <c r="MM12" s="77"/>
+      <c r="MN12" s="77"/>
+      <c r="MO12" s="77"/>
+      <c r="MP12" s="77"/>
+      <c r="MQ12" s="77"/>
+      <c r="MR12" s="77"/>
+      <c r="MS12" s="77"/>
+      <c r="MT12" s="77"/>
+      <c r="MU12" s="77"/>
+      <c r="MV12" s="77"/>
+      <c r="MW12" s="77"/>
+      <c r="MX12" s="77"/>
+      <c r="MY12" s="77"/>
+      <c r="MZ12" s="77"/>
+      <c r="NA12" s="77"/>
+      <c r="NB12" s="77"/>
+      <c r="NC12" s="77"/>
+      <c r="ND12" s="77"/>
+      <c r="NE12" s="77"/>
+      <c r="NF12" s="77"/>
+      <c r="NG12" s="77"/>
+      <c r="NH12" s="77"/>
+      <c r="NI12" s="77"/>
+      <c r="NJ12" s="77"/>
+      <c r="NK12" s="77"/>
+      <c r="NL12" s="77"/>
+      <c r="NM12" s="77"/>
+      <c r="NN12" s="77"/>
+      <c r="NO12" s="77"/>
+      <c r="NP12" s="77"/>
+      <c r="NQ12" s="77"/>
+      <c r="NR12" s="77"/>
+      <c r="NS12" s="77"/>
+      <c r="NT12" s="77"/>
+      <c r="NU12" s="77"/>
+      <c r="NV12" s="77"/>
+      <c r="NW12" s="77"/>
+      <c r="NX12" s="77"/>
+      <c r="NY12" s="77"/>
+      <c r="NZ12" s="77"/>
+      <c r="OA12" s="77"/>
+      <c r="OB12" s="77"/>
+      <c r="OC12" s="77"/>
+      <c r="OD12" s="77"/>
+      <c r="OE12" s="77"/>
+      <c r="OF12" s="77"/>
+      <c r="OG12" s="77"/>
+      <c r="OH12" s="77"/>
+      <c r="OI12" s="77"/>
+      <c r="OJ12" s="77"/>
+      <c r="OK12" s="77"/>
+      <c r="OL12" s="77"/>
+      <c r="OM12" s="77"/>
+      <c r="ON12" s="77"/>
+      <c r="OO12" s="77"/>
+      <c r="OP12" s="77"/>
+      <c r="OQ12" s="77"/>
+      <c r="OR12" s="77"/>
+      <c r="OS12" s="77"/>
+      <c r="OT12" s="77"/>
+      <c r="OU12" s="77"/>
+      <c r="OV12" s="77"/>
+      <c r="OW12" s="77"/>
+      <c r="OX12" s="77"/>
+      <c r="OY12" s="77"/>
+      <c r="OZ12" s="77"/>
+      <c r="PA12" s="77"/>
+      <c r="PB12" s="77"/>
+      <c r="PC12" s="77"/>
+      <c r="PD12" s="77"/>
+      <c r="PE12" s="77"/>
+      <c r="PF12" s="77"/>
+      <c r="PG12" s="77"/>
+      <c r="PH12" s="77"/>
+      <c r="PI12" s="77"/>
+      <c r="PJ12" s="77"/>
+      <c r="PK12" s="77"/>
+      <c r="PL12" s="77"/>
+      <c r="PM12" s="77"/>
+      <c r="PN12" s="77"/>
+      <c r="PO12" s="77"/>
+      <c r="PP12" s="77"/>
+      <c r="PQ12" s="77"/>
+      <c r="PR12" s="77"/>
+      <c r="PS12" s="77"/>
+      <c r="PT12" s="77"/>
+      <c r="PU12" s="77"/>
+      <c r="PV12" s="77"/>
+      <c r="PW12" s="77"/>
+      <c r="PX12" s="77"/>
+      <c r="PY12" s="77"/>
+      <c r="PZ12" s="77"/>
+      <c r="QA12" s="77"/>
+      <c r="QB12" s="77"/>
+      <c r="QC12" s="77"/>
+      <c r="QD12" s="77"/>
+      <c r="QE12" s="77"/>
+      <c r="QF12" s="77"/>
+      <c r="QG12" s="77"/>
+      <c r="QH12" s="77"/>
+      <c r="QI12" s="77"/>
+      <c r="QJ12" s="77"/>
+      <c r="QK12" s="77"/>
+      <c r="QL12" s="77"/>
+      <c r="QM12" s="77"/>
+      <c r="QN12" s="77"/>
+      <c r="QO12" s="77"/>
+      <c r="QP12" s="77"/>
+      <c r="QQ12" s="77"/>
+      <c r="QR12" s="77"/>
+      <c r="QS12" s="77"/>
+      <c r="QT12" s="77"/>
+      <c r="QU12" s="77"/>
+      <c r="QV12" s="77"/>
+      <c r="QW12" s="77"/>
+      <c r="QX12" s="77"/>
+      <c r="QY12" s="77"/>
+      <c r="QZ12" s="77"/>
+      <c r="RA12" s="77"/>
+      <c r="RB12" s="77"/>
+      <c r="RC12" s="77"/>
+      <c r="RD12" s="77"/>
+      <c r="RE12" s="77"/>
+      <c r="RF12" s="77"/>
+      <c r="RG12" s="77"/>
+      <c r="RH12" s="77"/>
+      <c r="RI12" s="77"/>
+      <c r="RJ12" s="77"/>
+      <c r="RK12" s="77"/>
+      <c r="RL12" s="77"/>
+      <c r="RM12" s="77"/>
+      <c r="RN12" s="77"/>
+      <c r="RO12" s="77"/>
+      <c r="RP12" s="77"/>
+      <c r="RQ12" s="77"/>
+      <c r="RR12" s="77"/>
+      <c r="RS12" s="77"/>
+      <c r="RT12" s="77"/>
+      <c r="RU12" s="77"/>
+      <c r="RV12" s="77"/>
+      <c r="RW12" s="77"/>
+      <c r="RX12" s="77"/>
+      <c r="RY12" s="77"/>
+      <c r="RZ12" s="77"/>
+      <c r="SA12" s="77"/>
+      <c r="SB12" s="77"/>
+      <c r="SC12" s="77"/>
+      <c r="SD12" s="77"/>
+      <c r="SE12" s="77"/>
+      <c r="SF12" s="77"/>
+      <c r="SG12" s="77"/>
+      <c r="SH12" s="77"/>
+      <c r="SI12" s="77"/>
+      <c r="SJ12" s="77"/>
+      <c r="SK12" s="77"/>
+      <c r="SL12" s="77"/>
+      <c r="SM12" s="77"/>
+      <c r="SN12" s="77"/>
+      <c r="SO12" s="77"/>
+      <c r="SP12" s="77"/>
+      <c r="SQ12" s="77"/>
+      <c r="SR12" s="77"/>
+      <c r="SS12" s="77"/>
+      <c r="ST12" s="77"/>
+      <c r="SU12" s="77"/>
+      <c r="SV12" s="77"/>
+      <c r="SW12" s="77"/>
+      <c r="SX12" s="77"/>
+      <c r="SY12" s="77"/>
+      <c r="SZ12" s="77"/>
+      <c r="TA12" s="77"/>
+      <c r="TB12" s="77"/>
+      <c r="TC12" s="77"/>
+      <c r="TD12" s="77"/>
+      <c r="TE12" s="77"/>
+      <c r="TF12" s="77"/>
+      <c r="TG12" s="77"/>
+      <c r="TH12" s="77"/>
+      <c r="TI12" s="77"/>
+      <c r="TJ12" s="77"/>
+      <c r="TK12" s="77"/>
+      <c r="TL12" s="77"/>
+      <c r="TM12" s="77"/>
+      <c r="TN12" s="77"/>
+      <c r="TO12" s="77"/>
+      <c r="TP12" s="77"/>
+      <c r="TQ12" s="77"/>
+      <c r="TR12" s="77"/>
+      <c r="TS12" s="77"/>
+      <c r="TT12" s="77"/>
+      <c r="TU12" s="77"/>
+      <c r="TV12" s="77"/>
+      <c r="TW12" s="77"/>
+      <c r="TX12" s="77"/>
+      <c r="TY12" s="77"/>
+      <c r="TZ12" s="77"/>
+      <c r="UA12" s="77"/>
+      <c r="UB12" s="77"/>
+      <c r="UC12" s="77"/>
+      <c r="UD12" s="77"/>
+      <c r="UE12" s="77"/>
+      <c r="UF12" s="77"/>
+      <c r="UG12" s="77"/>
+      <c r="UH12" s="77"/>
+      <c r="UI12" s="77"/>
+      <c r="UJ12" s="77"/>
+      <c r="UK12" s="77"/>
+      <c r="UL12" s="77"/>
+      <c r="UM12" s="77"/>
+      <c r="UN12" s="77"/>
+      <c r="UO12" s="77"/>
+      <c r="UP12" s="77"/>
+      <c r="UQ12" s="77"/>
+      <c r="UR12" s="77"/>
+      <c r="US12" s="77"/>
+      <c r="UT12" s="77"/>
+      <c r="UU12" s="77"/>
+      <c r="UV12" s="77"/>
+      <c r="UW12" s="77"/>
+      <c r="UX12" s="77"/>
+      <c r="UY12" s="77"/>
+      <c r="UZ12" s="77"/>
+      <c r="VA12" s="77"/>
+      <c r="VB12" s="77"/>
+      <c r="VC12" s="77"/>
+      <c r="VD12" s="77"/>
+      <c r="VE12" s="77"/>
+      <c r="VF12" s="77"/>
+      <c r="VG12" s="77"/>
+      <c r="VH12" s="77"/>
+      <c r="VI12" s="77"/>
+      <c r="VJ12" s="77"/>
+      <c r="VK12" s="77"/>
+      <c r="VL12" s="77"/>
+      <c r="VM12" s="77"/>
+      <c r="VN12" s="77"/>
+      <c r="VO12" s="77"/>
+      <c r="VP12" s="77"/>
+      <c r="VQ12" s="77"/>
+      <c r="VR12" s="77"/>
+      <c r="VS12" s="77"/>
+      <c r="VT12" s="77"/>
+      <c r="VU12" s="77"/>
+      <c r="VV12" s="77"/>
+      <c r="VW12" s="77"/>
+      <c r="VX12" s="77"/>
+      <c r="VY12" s="77"/>
+      <c r="VZ12" s="77"/>
+      <c r="WA12" s="77"/>
+      <c r="WB12" s="77"/>
+      <c r="WC12" s="77"/>
+      <c r="WD12" s="77"/>
+      <c r="WE12" s="77"/>
+      <c r="WF12" s="77"/>
+      <c r="WG12" s="77"/>
+      <c r="WH12" s="77"/>
+      <c r="WI12" s="77"/>
+      <c r="WJ12" s="77"/>
+      <c r="WK12" s="77"/>
+      <c r="WL12" s="77"/>
+      <c r="WM12" s="77"/>
+      <c r="WN12" s="77"/>
+      <c r="WO12" s="77"/>
+      <c r="WP12" s="77"/>
+      <c r="WQ12" s="77"/>
+      <c r="WR12" s="77"/>
+      <c r="WS12" s="77"/>
+      <c r="WT12" s="77"/>
+      <c r="WU12" s="77"/>
+      <c r="WV12" s="77"/>
+      <c r="WW12" s="77"/>
+      <c r="WX12" s="77"/>
+      <c r="WY12" s="77"/>
+      <c r="WZ12" s="77"/>
+      <c r="XA12" s="77"/>
+      <c r="XB12" s="77"/>
+      <c r="XC12" s="77"/>
+      <c r="XD12" s="77"/>
+      <c r="XE12" s="77"/>
+      <c r="XF12" s="77"/>
+      <c r="XG12" s="77"/>
+      <c r="XH12" s="77"/>
+      <c r="XI12" s="77"/>
+      <c r="XJ12" s="77"/>
+      <c r="XK12" s="77"/>
+      <c r="XL12" s="77"/>
+      <c r="XM12" s="77"/>
+      <c r="XN12" s="77"/>
+      <c r="XO12" s="77"/>
+      <c r="XP12" s="77"/>
+      <c r="XQ12" s="77"/>
+      <c r="XR12" s="77"/>
+      <c r="XS12" s="77"/>
+      <c r="XT12" s="77"/>
+      <c r="XU12" s="77"/>
+      <c r="XV12" s="77"/>
+      <c r="XW12" s="77"/>
+      <c r="XX12" s="77"/>
+      <c r="XY12" s="77"/>
+      <c r="XZ12" s="77"/>
+      <c r="YA12" s="77"/>
+      <c r="YB12" s="77"/>
+      <c r="YC12" s="77"/>
+      <c r="YD12" s="77"/>
+      <c r="YE12" s="77"/>
+      <c r="YF12" s="77"/>
+      <c r="YG12" s="77"/>
+      <c r="YH12" s="77"/>
+      <c r="YI12" s="77"/>
+      <c r="YJ12" s="77"/>
+      <c r="YK12" s="77"/>
+      <c r="YL12" s="77"/>
+      <c r="YM12" s="77"/>
+      <c r="YN12" s="77"/>
+      <c r="YO12" s="77"/>
+      <c r="YP12" s="77"/>
+      <c r="YQ12" s="77"/>
+      <c r="YR12" s="77"/>
+      <c r="YS12" s="77"/>
+      <c r="YT12" s="77"/>
+      <c r="YU12" s="77"/>
+      <c r="YV12" s="77"/>
+      <c r="YW12" s="77"/>
+      <c r="YX12" s="77"/>
+      <c r="YY12" s="77"/>
+      <c r="YZ12" s="77"/>
+      <c r="ZA12" s="77"/>
+      <c r="ZB12" s="77"/>
+      <c r="ZC12" s="77"/>
+      <c r="ZD12" s="77"/>
+      <c r="ZE12" s="77"/>
+      <c r="ZF12" s="77"/>
+      <c r="ZG12" s="77"/>
+      <c r="ZH12" s="77"/>
+      <c r="ZI12" s="77"/>
+      <c r="ZJ12" s="77"/>
+      <c r="ZK12" s="77"/>
+      <c r="ZL12" s="77"/>
+      <c r="ZM12" s="77"/>
+      <c r="ZN12" s="77"/>
+      <c r="ZO12" s="77"/>
+      <c r="ZP12" s="77"/>
+      <c r="ZQ12" s="77"/>
+      <c r="ZR12" s="77"/>
+      <c r="ZS12" s="77"/>
+      <c r="ZT12" s="77"/>
+      <c r="ZU12" s="77"/>
+      <c r="ZV12" s="77"/>
+      <c r="ZW12" s="77"/>
+      <c r="ZX12" s="77"/>
+      <c r="ZY12" s="77"/>
+      <c r="ZZ12" s="77"/>
+      <c r="AAA12" s="77"/>
+      <c r="AAB12" s="77"/>
+      <c r="AAC12" s="77"/>
+      <c r="AAD12" s="77"/>
+      <c r="AAE12" s="77"/>
+      <c r="AAF12" s="77"/>
+      <c r="AAG12" s="77"/>
+      <c r="AAH12" s="77"/>
+      <c r="AAI12" s="77"/>
+      <c r="AAJ12" s="77"/>
+      <c r="AAK12" s="77"/>
+      <c r="AAL12" s="77"/>
+      <c r="AAM12" s="77"/>
+      <c r="AAN12" s="77"/>
+      <c r="AAO12" s="77"/>
+      <c r="AAP12" s="77"/>
+      <c r="AAQ12" s="77"/>
+      <c r="AAR12" s="77"/>
+      <c r="AAS12" s="77"/>
+      <c r="AAT12" s="77"/>
+      <c r="AAU12" s="77"/>
+      <c r="AAV12" s="77"/>
+      <c r="AAW12" s="77"/>
+      <c r="AAX12" s="77"/>
+      <c r="AAY12" s="77"/>
+      <c r="AAZ12" s="77"/>
+      <c r="ABA12" s="77"/>
+      <c r="ABB12" s="77"/>
+      <c r="ABC12" s="77"/>
+      <c r="ABD12" s="77"/>
+      <c r="ABE12" s="77"/>
+      <c r="ABF12" s="77"/>
+      <c r="ABG12" s="77"/>
+      <c r="ABH12" s="77"/>
+      <c r="ABI12" s="77"/>
+      <c r="ABJ12" s="77"/>
+      <c r="ABK12" s="77"/>
+      <c r="ABL12" s="77"/>
+      <c r="ABM12" s="77"/>
+      <c r="ABN12" s="77"/>
+      <c r="ABO12" s="77"/>
+      <c r="ABP12" s="77"/>
+      <c r="ABQ12" s="77"/>
+      <c r="ABR12" s="77"/>
+      <c r="ABS12" s="77"/>
+      <c r="ABT12" s="77"/>
+      <c r="ABU12" s="77"/>
+      <c r="ABV12" s="77"/>
+      <c r="ABW12" s="77"/>
+      <c r="ABX12" s="77"/>
+      <c r="ABY12" s="77"/>
+      <c r="ABZ12" s="77"/>
+      <c r="ACA12" s="77"/>
+      <c r="ACB12" s="77"/>
+      <c r="ACC12" s="77"/>
+      <c r="ACD12" s="77"/>
+      <c r="ACE12" s="77"/>
+      <c r="ACF12" s="77"/>
+      <c r="ACG12" s="77"/>
+      <c r="ACH12" s="77"/>
+      <c r="ACI12" s="77"/>
+      <c r="ACJ12" s="77"/>
+      <c r="ACK12" s="77"/>
+      <c r="ACL12" s="77"/>
+      <c r="ACM12" s="77"/>
+      <c r="ACN12" s="77"/>
+      <c r="ACO12" s="77"/>
+      <c r="ACP12" s="77"/>
+      <c r="ACQ12" s="77"/>
+      <c r="ACR12" s="77"/>
+      <c r="ACS12" s="77"/>
+      <c r="ACT12" s="77"/>
+      <c r="ACU12" s="77"/>
+      <c r="ACV12" s="77"/>
+      <c r="ACW12" s="77"/>
+      <c r="ACX12" s="77"/>
+      <c r="ACY12" s="77"/>
+      <c r="ACZ12" s="77"/>
+      <c r="ADA12" s="77"/>
+      <c r="ADB12" s="77"/>
+      <c r="ADC12" s="77"/>
+      <c r="ADD12" s="77"/>
+      <c r="ADE12" s="77"/>
+      <c r="ADF12" s="77"/>
+      <c r="ADG12" s="77"/>
+      <c r="ADH12" s="77"/>
+      <c r="ADI12" s="77"/>
+      <c r="ADJ12" s="77"/>
+      <c r="ADK12" s="77"/>
+      <c r="ADL12" s="77"/>
+      <c r="ADM12" s="77"/>
+      <c r="ADN12" s="77"/>
+      <c r="ADO12" s="77"/>
+      <c r="ADP12" s="77"/>
+      <c r="ADQ12" s="77"/>
+      <c r="ADR12" s="77"/>
+      <c r="ADS12" s="77"/>
+      <c r="ADT12" s="77"/>
+      <c r="ADU12" s="77"/>
+      <c r="ADV12" s="77"/>
+      <c r="ADW12" s="77"/>
+      <c r="ADX12" s="77"/>
+      <c r="ADY12" s="77"/>
+      <c r="ADZ12" s="77"/>
+      <c r="AEA12" s="77"/>
+      <c r="AEB12" s="77"/>
+      <c r="AEC12" s="77"/>
+      <c r="AED12" s="77"/>
+      <c r="AEE12" s="77"/>
+      <c r="AEF12" s="77"/>
+      <c r="AEG12" s="77"/>
+      <c r="AEH12" s="77"/>
+      <c r="AEI12" s="77"/>
+      <c r="AEJ12" s="77"/>
+      <c r="AEK12" s="77"/>
+      <c r="AEL12" s="77"/>
+      <c r="AEM12" s="77"/>
+      <c r="AEN12" s="77"/>
+      <c r="AEO12" s="77"/>
+      <c r="AEP12" s="77"/>
+      <c r="AEQ12" s="77"/>
+      <c r="AER12" s="77"/>
+      <c r="AES12" s="77"/>
+      <c r="AET12" s="77"/>
+      <c r="AEU12" s="77"/>
+      <c r="AEV12" s="77"/>
+      <c r="AEW12" s="77"/>
+      <c r="AEX12" s="77"/>
+      <c r="AEY12" s="77"/>
+      <c r="AEZ12" s="77"/>
+      <c r="AFA12" s="77"/>
+      <c r="AFB12" s="77"/>
+      <c r="AFC12" s="77"/>
+      <c r="AFD12" s="77"/>
+      <c r="AFE12" s="77"/>
+      <c r="AFF12" s="77"/>
+      <c r="AFG12" s="77"/>
+      <c r="AFH12" s="77"/>
+      <c r="AFI12" s="77"/>
+      <c r="AFJ12" s="77"/>
+      <c r="AFK12" s="77"/>
+      <c r="AFL12" s="77"/>
+      <c r="AFM12" s="77"/>
+      <c r="AFN12" s="77"/>
+      <c r="AFO12" s="77"/>
+      <c r="AFP12" s="77"/>
+      <c r="AFQ12" s="77"/>
+      <c r="AFR12" s="77"/>
+      <c r="AFS12" s="77"/>
+      <c r="AFT12" s="77"/>
+      <c r="AFU12" s="77"/>
+      <c r="AFV12" s="77"/>
+      <c r="AFW12" s="77"/>
+      <c r="AFX12" s="77"/>
+      <c r="AFY12" s="77"/>
+      <c r="AFZ12" s="77"/>
+      <c r="AGA12" s="77"/>
+      <c r="AGB12" s="77"/>
+      <c r="AGC12" s="77"/>
+      <c r="AGD12" s="77"/>
+      <c r="AGE12" s="77"/>
+      <c r="AGF12" s="77"/>
+      <c r="AGG12" s="77"/>
+      <c r="AGH12" s="77"/>
+      <c r="AGI12" s="77"/>
+      <c r="AGJ12" s="77"/>
+      <c r="AGK12" s="77"/>
+      <c r="AGL12" s="77"/>
+      <c r="AGM12" s="77"/>
+      <c r="AGN12" s="77"/>
+      <c r="AGO12" s="77"/>
+      <c r="AGP12" s="77"/>
+      <c r="AGQ12" s="77"/>
+      <c r="AGR12" s="77"/>
+      <c r="AGS12" s="77"/>
+      <c r="AGT12" s="77"/>
+      <c r="AGU12" s="77"/>
+      <c r="AGV12" s="77"/>
+      <c r="AGW12" s="77"/>
+      <c r="AGX12" s="77"/>
+      <c r="AGY12" s="77"/>
+      <c r="AGZ12" s="77"/>
+      <c r="AHA12" s="77"/>
+      <c r="AHB12" s="77"/>
+      <c r="AHC12" s="77"/>
+      <c r="AHD12" s="77"/>
+      <c r="AHE12" s="77"/>
+      <c r="AHF12" s="77"/>
+      <c r="AHG12" s="77"/>
+      <c r="AHH12" s="77"/>
+      <c r="AHI12" s="77"/>
+      <c r="AHJ12" s="77"/>
+      <c r="AHK12" s="77"/>
+      <c r="AHL12" s="77"/>
+      <c r="AHM12" s="77"/>
+      <c r="AHN12" s="77"/>
+      <c r="AHO12" s="77"/>
+      <c r="AHP12" s="77"/>
+      <c r="AHQ12" s="77"/>
+      <c r="AHR12" s="77"/>
+      <c r="AHS12" s="77"/>
+      <c r="AHT12" s="77"/>
+      <c r="AHU12" s="77"/>
+      <c r="AHV12" s="77"/>
+      <c r="AHW12" s="77"/>
+      <c r="AHX12" s="77"/>
+      <c r="AHY12" s="77"/>
+      <c r="AHZ12" s="77"/>
+      <c r="AIA12" s="77"/>
+      <c r="AIB12" s="77"/>
+      <c r="AIC12" s="77"/>
+      <c r="AID12" s="77"/>
+      <c r="AIE12" s="77"/>
+      <c r="AIF12" s="77"/>
+      <c r="AIG12" s="77"/>
+      <c r="AIH12" s="77"/>
+      <c r="AII12" s="77"/>
+      <c r="AIJ12" s="77"/>
+      <c r="AIK12" s="77"/>
+      <c r="AIL12" s="77"/>
+      <c r="AIM12" s="77"/>
+      <c r="AIN12" s="77"/>
+      <c r="AIO12" s="77"/>
+      <c r="AIP12" s="77"/>
+      <c r="AIQ12" s="77"/>
+      <c r="AIR12" s="77"/>
+      <c r="AIS12" s="77"/>
+      <c r="AIT12" s="77"/>
+      <c r="AIU12" s="77"/>
+      <c r="AIV12" s="77"/>
+      <c r="AIW12" s="77"/>
+      <c r="AIX12" s="77"/>
+      <c r="AIY12" s="77"/>
+      <c r="AIZ12" s="77"/>
+      <c r="AJA12" s="77"/>
+      <c r="AJB12" s="77"/>
+      <c r="AJC12" s="77"/>
+      <c r="AJD12" s="77"/>
+      <c r="AJE12" s="77"/>
+      <c r="AJF12" s="77"/>
+      <c r="AJG12" s="77"/>
+      <c r="AJH12" s="77"/>
+      <c r="AJI12" s="77"/>
+      <c r="AJJ12" s="77"/>
+      <c r="AJK12" s="77"/>
+      <c r="AJL12" s="77"/>
+      <c r="AJM12" s="77"/>
+      <c r="AJN12" s="77"/>
+      <c r="AJO12" s="77"/>
+      <c r="AJP12" s="77"/>
+      <c r="AJQ12" s="77"/>
+      <c r="AJR12" s="77"/>
+      <c r="AJS12" s="77"/>
+      <c r="AJT12" s="77"/>
+      <c r="AJU12" s="77"/>
+      <c r="AJV12" s="77"/>
+      <c r="AJW12" s="77"/>
+      <c r="AJX12" s="77"/>
+      <c r="AJY12" s="77"/>
+      <c r="AJZ12" s="77"/>
+      <c r="AKA12" s="77"/>
+      <c r="AKB12" s="77"/>
+      <c r="AKC12" s="77"/>
+      <c r="AKD12" s="77"/>
+      <c r="AKE12" s="77"/>
+      <c r="AKF12" s="77"/>
+      <c r="AKG12" s="77"/>
+      <c r="AKH12" s="77"/>
+      <c r="AKI12" s="77"/>
+      <c r="AKJ12" s="77"/>
+      <c r="AKK12" s="77"/>
+      <c r="AKL12" s="77"/>
+      <c r="AKM12" s="77"/>
+      <c r="AKN12" s="77"/>
+      <c r="AKO12" s="77"/>
+      <c r="AKP12" s="77"/>
+      <c r="AKQ12" s="77"/>
+      <c r="AKR12" s="77"/>
+      <c r="AKS12" s="77"/>
+      <c r="AKT12" s="77"/>
+      <c r="AKU12" s="77"/>
+      <c r="AKV12" s="77"/>
+      <c r="AKW12" s="77"/>
+      <c r="AKX12" s="77"/>
+      <c r="AKY12" s="77"/>
+      <c r="AKZ12" s="77"/>
+      <c r="ALA12" s="77"/>
+      <c r="ALB12" s="77"/>
+      <c r="ALC12" s="77"/>
+      <c r="ALD12" s="77"/>
+      <c r="ALE12" s="77"/>
+      <c r="ALF12" s="77"/>
+      <c r="ALG12" s="77"/>
+      <c r="ALH12" s="77"/>
+      <c r="ALI12" s="77"/>
+      <c r="ALJ12" s="77"/>
+      <c r="ALK12" s="77"/>
+      <c r="ALL12" s="77"/>
+      <c r="ALM12" s="77"/>
+      <c r="ALN12" s="77"/>
+      <c r="ALO12" s="77"/>
+      <c r="ALP12" s="77"/>
+      <c r="ALQ12" s="77"/>
+      <c r="ALR12" s="77"/>
+      <c r="ALS12" s="77"/>
+      <c r="ALT12" s="77"/>
+      <c r="ALU12" s="77"/>
+      <c r="ALV12" s="77"/>
+      <c r="ALW12" s="77"/>
+      <c r="ALX12" s="77"/>
+      <c r="ALY12" s="77"/>
+      <c r="ALZ12" s="77"/>
+      <c r="AMA12" s="77"/>
+      <c r="AMB12" s="77"/>
+      <c r="AMC12" s="77"/>
+      <c r="AMD12" s="77"/>
+      <c r="AME12" s="77"/>
+      <c r="AMF12" s="77"/>
+      <c r="AMG12" s="77"/>
+      <c r="AMH12" s="77"/>
+      <c r="AMI12" s="77"/>
+      <c r="AMJ12" s="77"/>
     </row>
     <row r="13" s="77" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="61"/>
@@ -19907,7 +24033,7 @@
   <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="19:19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.65234375" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20483,7 +24609,7 @@
   <dimension ref="A1:AF22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="1" sqref="19:19 E6"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21059,7 +25185,7 @@
   <dimension ref="A1:AF19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="1" sqref="19:19 E17"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.37109375" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21658,11 +25784,11 @@
   <dimension ref="A1:AG25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="D12" activeCellId="1" sqref="19:19 D12"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fix: :bug: fix structure definition typo
</commit_message>
<xml_diff>
--- a/input/l2/global.xlsx
+++ b/input/l2/global.xlsx
@@ -8155,7 +8155,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.37109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20223,13 +20223,15 @@
   </sheetPr>
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="1" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="32.03"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24723,7 +24725,7 @@
   </sheetPr>
   <dimension ref="A1:AF22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>